<commit_message>
Starting with Literature Review section FL Algorithms.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E15FE42C-CED5-43DE-8859-1A0CDE09E4F4}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51DCA11D-2FE7-4385-9F91-D8A98C84BEAD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
     <sheet name="T.2.3.3." sheetId="2" r:id="rId2"/>
     <sheet name="T.3.1." sheetId="3" r:id="rId3"/>
+    <sheet name="T.3.2." sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$K$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
   <si>
     <t>FL</t>
   </si>
@@ -148,12 +150,6 @@
     <t xml:space="preserve">Distributed Machine Learning </t>
   </si>
   <si>
-    <t>IBMFL</t>
-  </si>
-  <si>
-    <t>IBM Federated Learning</t>
-  </si>
-  <si>
     <t>API</t>
   </si>
   <si>
@@ -272,6 +268,45 @@
   </si>
   <si>
     <t>Normalised Contributors</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>SDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Development Kit </t>
+  </si>
+  <si>
+    <t>Nvidia Flare</t>
+  </si>
+  <si>
+    <t>DLT</t>
+  </si>
+  <si>
+    <t>Distributed Ledger Technology</t>
+  </si>
+  <si>
+    <t>Algorithms Used</t>
+  </si>
+  <si>
+    <t>FedAvg and  SecureBoost</t>
+  </si>
+  <si>
+    <t>FedAvg, FedProx and FedMA</t>
+  </si>
+  <si>
+    <t>FedAvg</t>
+  </si>
+  <si>
+    <t>FedAvg, SecureBoost and Custom FL Algorithms</t>
+  </si>
+  <si>
+    <t>FedAvg, FedProx, and Custom FL Algorithms</t>
+  </si>
+  <si>
+    <t>FedAvg and Custom FL Algorithms</t>
   </si>
 </sst>
 </file>
@@ -279,7 +314,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -381,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -398,7 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -406,9 +441,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -419,13 +451,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,10 +836,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -802,95 +852,111 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
-    <sortCondition ref="A2:A13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -974,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C96B4BA-4EFD-4BFD-AC4C-1FFB139FC407}">
   <dimension ref="C4:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,63 +1066,63 @@
   <sheetData>
     <row r="4" spans="3:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="V4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5">
         <v>9373</v>
@@ -1068,26 +1134,26 @@
         <v>429</v>
       </c>
       <c r="G5" s="6">
-        <f>(D5-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" ref="G5:G14" si="0">(D5-$D$18)/($D$19-$D$18)</f>
         <v>1</v>
       </c>
       <c r="H5" s="6">
-        <f>(E5-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" ref="H5:H14" si="1">(E5-$E$18)/($E$19-$E$18)</f>
         <v>1</v>
       </c>
       <c r="I5" s="6">
-        <f>(F5-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" ref="I5:I14" si="2">(F5-$F$18)/($F$19-$F$18)</f>
         <v>1</v>
       </c>
       <c r="J5" s="6">
-        <f>(G5+H5+I5)/3</f>
+        <f t="shared" ref="J5:J14" si="3">(G5+H5+I5)/3</f>
         <v>1</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P5" s="13">
         <v>1</v>
@@ -1111,12 +1177,12 @@
         <v>429</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5">
         <v>5595</v>
@@ -1128,26 +1194,26 @@
         <v>86</v>
       </c>
       <c r="G6" s="6">
-        <f>(D6-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>0.58510871952558752</v>
       </c>
       <c r="H6" s="6">
-        <f>(E6-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>0.77040816326530615</v>
       </c>
       <c r="I6" s="6">
-        <f>(F6-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>0.18333333333333332</v>
       </c>
       <c r="J6" s="6">
-        <f>(G6+H6+I6)/3</f>
+        <f t="shared" si="3"/>
         <v>0.51295007204140897</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P6" s="13">
         <v>0.51295007204140897</v>
@@ -1171,12 +1237,12 @@
         <v>86</v>
       </c>
       <c r="W6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="5">
         <v>4512</v>
@@ -1188,26 +1254,26 @@
         <v>127</v>
       </c>
       <c r="G7" s="6">
-        <f>(D7-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>0.46617614759499232</v>
       </c>
       <c r="H7" s="6">
-        <f>(E7-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>0.38724489795918365</v>
       </c>
       <c r="I7" s="6">
-        <f>(F7-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>0.28095238095238095</v>
       </c>
       <c r="J7" s="6">
-        <f>(G7+H7+I7)/3</f>
+        <f t="shared" si="3"/>
         <v>0.37812447550218559</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P7" s="13">
         <v>0.37812447550218559</v>
@@ -1231,12 +1297,12 @@
         <v>127</v>
       </c>
       <c r="W7" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" s="5">
         <v>4113</v>
@@ -1248,26 +1314,26 @@
         <v>66</v>
       </c>
       <c r="G8" s="6">
-        <f>(D8-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>0.42235888425214146</v>
       </c>
       <c r="H8" s="6">
-        <f>(E8-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>0.37704081632653064</v>
       </c>
       <c r="I8" s="6">
-        <f>(F8-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>0.1357142857142857</v>
       </c>
       <c r="J8" s="6">
-        <f>(G8+H8+I8)/3</f>
+        <f t="shared" si="3"/>
         <v>0.31170466209765263</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P8" s="13">
         <v>0.31170466209765263</v>
@@ -1291,7 +1357,7 @@
         <v>66</v>
       </c>
       <c r="W8" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.3">
@@ -1308,23 +1374,23 @@
         <v>108</v>
       </c>
       <c r="G9" s="6">
-        <f>(D9-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>0.22303975400834614</v>
       </c>
       <c r="H9" s="6">
-        <f>(E9-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>0.27857142857142858</v>
       </c>
       <c r="I9" s="6">
-        <f>(F9-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>0.23571428571428571</v>
       </c>
       <c r="J9" s="6">
-        <f>(G9+H9+I9)/3</f>
+        <f t="shared" si="3"/>
         <v>0.24577515609802014</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>9</v>
@@ -1351,12 +1417,12 @@
         <v>108</v>
       </c>
       <c r="W9" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5">
         <v>687</v>
@@ -1368,26 +1434,26 @@
         <v>83</v>
       </c>
       <c r="G10" s="6">
-        <f>(D10-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>4.6123435097737753E-2</v>
       </c>
       <c r="H10" s="6">
-        <f>(E10-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>7.5510204081632656E-2</v>
       </c>
       <c r="I10" s="6">
-        <f>(F10-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>0.1761904761904762</v>
       </c>
       <c r="J10" s="6">
-        <f>(G10+H10+I10)/3</f>
+        <f t="shared" si="3"/>
         <v>9.9274705123282195E-2</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P10" s="13">
         <v>9.9274705123282195E-2</v>
@@ -1411,12 +1477,12 @@
         <v>83</v>
       </c>
       <c r="W10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="5">
         <v>578</v>
@@ -1428,26 +1494,26 @@
         <v>40</v>
       </c>
       <c r="G11" s="6">
-        <f>(D11-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>3.4153305512848668E-2</v>
       </c>
       <c r="H11" s="6">
-        <f>(E11-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>6.4285714285714279E-2</v>
       </c>
       <c r="I11" s="6">
-        <f>(F11-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>7.3809523809523811E-2</v>
       </c>
       <c r="J11" s="6">
-        <f>(G11+H11+I11)/3</f>
+        <f t="shared" si="3"/>
         <v>5.7416181202695593E-2</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P11" s="13">
         <v>5.7416181202695593E-2</v>
@@ -1471,12 +1537,12 @@
         <v>40</v>
       </c>
       <c r="W11" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="5">
         <v>495</v>
@@ -1488,26 +1554,26 @@
         <v>25</v>
       </c>
       <c r="G12" s="6">
-        <f>(D12-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>2.5038436195914782E-2</v>
       </c>
       <c r="H12" s="6">
-        <f>(E12-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>4.4897959183673466E-2</v>
       </c>
       <c r="I12" s="6">
-        <f>(F12-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>3.8095238095238099E-2</v>
       </c>
       <c r="J12" s="6">
-        <f>(G12+H12+I12)/3</f>
+        <f t="shared" si="3"/>
         <v>3.601054449160878E-2</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P12" s="13">
         <v>3.601054449160878E-2</v>
@@ -1531,12 +1597,12 @@
         <v>25</v>
       </c>
       <c r="W12" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="5">
         <v>267</v>
@@ -1548,26 +1614,26 @@
         <v>36</v>
       </c>
       <c r="G13" s="6">
-        <f>(D13-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="6">
-        <f>(E13-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I13" s="6">
-        <f>(F13-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>6.4285714285714279E-2</v>
       </c>
       <c r="J13" s="6">
-        <f>(G13+H13+I13)/3</f>
+        <f t="shared" si="3"/>
         <v>2.1428571428571425E-2</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P13" s="13">
         <v>2.1428571428571425E-2</v>
@@ -1591,12 +1657,12 @@
         <v>36</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="3:23" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="5">
         <v>501</v>
@@ -1608,26 +1674,26 @@
         <v>9</v>
       </c>
       <c r="G14" s="6">
-        <f>(D14-$D$18)/($D$19-$D$18)</f>
+        <f t="shared" si="0"/>
         <v>2.5697342411596748E-2</v>
       </c>
       <c r="H14" s="6">
-        <f>(E14-$E$18)/($E$19-$E$18)</f>
+        <f t="shared" si="1"/>
         <v>2.6530612244897958E-2</v>
       </c>
       <c r="I14" s="6">
-        <f>(F14-$F$18)/($F$19-$F$18)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J14" s="6">
-        <f>(G14+H14+I14)/3</f>
+        <f t="shared" si="3"/>
         <v>1.7409318218831567E-2</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P14" s="13">
         <v>1.7409318218831567E-2</v>
@@ -1651,64 +1717,64 @@
         <v>9</v>
       </c>
       <c r="W14" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="O15" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
+      <c r="O15" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <f>MIN(D5:D14)</f>
         <v>267</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:F18" si="0">MIN(E5:E14)</f>
+        <f t="shared" ref="E18:F18" si="4">MIN(E5:E14)</f>
         <v>33</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19">
         <f>MAX(D5:D14)</f>
         <v>9373</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19:F19" si="1">MAX(E5:E14)</f>
+        <f t="shared" ref="E19:F19" si="5">MAX(E5:E14)</f>
         <v>1993</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>429</v>
       </c>
     </row>
@@ -1717,6 +1783,163 @@
     <mergeCell ref="C15:K15"/>
     <mergeCell ref="O15:W15"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="W12" r:id="rId1" xr:uid="{7682326C-FF86-4F21-8EBC-858C20C28CA6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF8C39F-1944-43A1-9D92-BE743AAE215C}">
+  <dimension ref="D3:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D5" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D6" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D14:F14"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1" xr:uid="{A4E9F801-A5C8-4DF3-A71D-8DC5325BCA54}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed section Federated Learning Algorithms.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51DCA11D-2FE7-4385-9F91-D8A98C84BEAD}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA8331D0-D892-4FBA-8994-5C0E0FF5CE2D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
     <sheet name="T.2.3.3." sheetId="2" r:id="rId2"/>
     <sheet name="T.3.1." sheetId="3" r:id="rId3"/>
     <sheet name="T.3.2." sheetId="4" r:id="rId4"/>
+    <sheet name="T.3.2.5." sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$K$4</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
   <si>
     <t>FL</t>
   </si>
@@ -307,6 +308,57 @@
   </si>
   <si>
     <t>FedAvg and Custom FL Algorithms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federated Averaging </t>
+  </si>
+  <si>
+    <t>FedMA</t>
+  </si>
+  <si>
+    <t>Federated Matched Averaging</t>
+  </si>
+  <si>
+    <t>CNN(s)</t>
+  </si>
+  <si>
+    <t>Convolutional Neural Network(s)</t>
+  </si>
+  <si>
+    <t>Long Short-Term Memory Networks</t>
+  </si>
+  <si>
+    <t>LSTM(s)</t>
+  </si>
+  <si>
+    <t>GBDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gradient Boosting Decision Trees </t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>FedProx</t>
+  </si>
+  <si>
+    <t>Constructs global models by matching and averaging hidden elements layer-wise, ensuring functional matching and reducing communication costs.</t>
+  </si>
+  <si>
+    <t>SecureBoost</t>
+  </si>
+  <si>
+    <t>Uses vertically partitioned data and privacy-preserving protocols to train gradient boosting models securely, ensuring data privacy through encryption.</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>A variation of FedAvg. Adds a proximal term to handle system and statistical heterogeneity, enabling non-uniform local computation and improving stability.</t>
+  </si>
+  <si>
+    <t>Trains models across multiple devices using Stochastic Gradient Descent, preserves centralized control, and reduces communication rounds.  It is efficient in non-IID data environments.</t>
   </si>
 </sst>
 </file>
@@ -416,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -442,6 +494,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -454,16 +519,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,8 +528,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,10 +546,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,119 +895,159 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
+    <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1155,28 +1246,28 @@
       <c r="O5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="9">
         <v>1</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="9">
         <v>1</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="9">
         <v>1</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="9">
         <v>1</v>
       </c>
-      <c r="T5" s="14">
+      <c r="T5" s="10">
         <v>9373</v>
       </c>
-      <c r="U5" s="14">
+      <c r="U5" s="10">
         <v>1993</v>
       </c>
-      <c r="V5" s="14">
+      <c r="V5" s="10">
         <v>429</v>
       </c>
-      <c r="W5" s="15" t="s">
+      <c r="W5" s="11" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1215,28 +1306,28 @@
       <c r="O6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="9">
         <v>0.51295007204140897</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="9">
         <v>0.58510871952558752</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="9">
         <v>0.77040816326530615</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="9">
         <v>0.18333333333333332</v>
       </c>
-      <c r="T6" s="14">
+      <c r="T6" s="10">
         <v>5595</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="10">
         <v>1543</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="10">
         <v>86</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="11" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1275,28 +1366,28 @@
       <c r="O7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="9">
         <v>0.37812447550218559</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="9">
         <v>0.46617614759499232</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="9">
         <v>0.38724489795918365</v>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="9">
         <v>0.28095238095238095</v>
       </c>
-      <c r="T7" s="14">
+      <c r="T7" s="10">
         <v>4512</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U7" s="10">
         <v>792</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V7" s="10">
         <v>127</v>
       </c>
-      <c r="W7" s="15" t="s">
+      <c r="W7" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1335,28 +1426,28 @@
       <c r="O8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="9">
         <v>0.31170466209765263</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="9">
         <v>0.42235888425214146</v>
       </c>
-      <c r="R8" s="13">
+      <c r="R8" s="9">
         <v>0.37704081632653064</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="9">
         <v>0.1357142857142857</v>
       </c>
-      <c r="T8" s="14">
+      <c r="T8" s="10">
         <v>4113</v>
       </c>
-      <c r="U8" s="14">
+      <c r="U8" s="10">
         <v>772</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8" s="10">
         <v>66</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="W8" s="11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1395,28 +1486,28 @@
       <c r="O9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="9">
         <v>0.24577515609802014</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="9">
         <v>0.22303975400834614</v>
       </c>
-      <c r="R9" s="13">
+      <c r="R9" s="9">
         <v>0.27857142857142858</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="9">
         <v>0.23571428571428571</v>
       </c>
-      <c r="T9" s="14">
+      <c r="T9" s="10">
         <v>2298</v>
       </c>
-      <c r="U9" s="14">
+      <c r="U9" s="10">
         <v>579</v>
       </c>
-      <c r="V9" s="14">
+      <c r="V9" s="10">
         <v>108</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="11" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1455,28 +1546,28 @@
       <c r="O10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="9">
         <v>9.9274705123282195E-2</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="9">
         <v>4.6123435097737753E-2</v>
       </c>
-      <c r="R10" s="13">
+      <c r="R10" s="9">
         <v>7.5510204081632656E-2</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="9">
         <v>0.1761904761904762</v>
       </c>
-      <c r="T10" s="14">
+      <c r="T10" s="10">
         <v>687</v>
       </c>
-      <c r="U10" s="14">
+      <c r="U10" s="10">
         <v>181</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="10">
         <v>83</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="W10" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1515,28 +1606,28 @@
       <c r="O11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="13">
+      <c r="P11" s="9">
         <v>5.7416181202695593E-2</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="9">
         <v>3.4153305512848668E-2</v>
       </c>
-      <c r="R11" s="13">
+      <c r="R11" s="9">
         <v>6.4285714285714279E-2</v>
       </c>
-      <c r="S11" s="13">
+      <c r="S11" s="9">
         <v>7.3809523809523811E-2</v>
       </c>
-      <c r="T11" s="14">
+      <c r="T11" s="10">
         <v>578</v>
       </c>
-      <c r="U11" s="14">
+      <c r="U11" s="10">
         <v>159</v>
       </c>
-      <c r="V11" s="14">
+      <c r="V11" s="10">
         <v>40</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="W11" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1575,28 +1666,28 @@
       <c r="O12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P12" s="9">
         <v>3.601054449160878E-2</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q12" s="9">
         <v>2.5038436195914782E-2</v>
       </c>
-      <c r="R12" s="13">
+      <c r="R12" s="9">
         <v>4.4897959183673466E-2</v>
       </c>
-      <c r="S12" s="13">
+      <c r="S12" s="9">
         <v>3.8095238095238099E-2</v>
       </c>
-      <c r="T12" s="14">
+      <c r="T12" s="10">
         <v>495</v>
       </c>
-      <c r="U12" s="14">
+      <c r="U12" s="10">
         <v>121</v>
       </c>
-      <c r="V12" s="14">
+      <c r="V12" s="10">
         <v>25</v>
       </c>
-      <c r="W12" s="15" t="s">
+      <c r="W12" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1635,28 +1726,28 @@
       <c r="O13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P13" s="13">
+      <c r="P13" s="9">
         <v>2.1428571428571425E-2</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="9">
         <v>0</v>
       </c>
-      <c r="R13" s="13">
+      <c r="R13" s="9">
         <v>0</v>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="9">
         <v>6.4285714285714279E-2</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="10">
         <v>267</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U13" s="10">
         <v>33</v>
       </c>
-      <c r="V13" s="14">
+      <c r="V13" s="10">
         <v>36</v>
       </c>
-      <c r="W13" s="15" t="s">
+      <c r="W13" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1695,54 +1786,54 @@
       <c r="O14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="9">
         <v>1.7409318218831567E-2</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="Q14" s="9">
         <v>2.5697342411596748E-2</v>
       </c>
-      <c r="R14" s="13">
+      <c r="R14" s="9">
         <v>2.6530612244897958E-2</v>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="9">
         <v>0</v>
       </c>
-      <c r="T14" s="14">
+      <c r="T14" s="10">
         <v>501</v>
       </c>
-      <c r="U14" s="14">
+      <c r="U14" s="10">
         <v>85</v>
       </c>
-      <c r="V14" s="14">
+      <c r="V14" s="10">
         <v>9</v>
       </c>
-      <c r="W14" s="15" t="s">
+      <c r="W14" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
-      <c r="O15" s="12" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="16"/>
+      <c r="O15" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -1794,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF8C39F-1944-43A1-9D92-BE743AAE215C}">
   <dimension ref="D3:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1817,121 +1908,121 @@
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1942,4 +2033,66 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3C5ED9-A3DC-46C6-9548-9775EC56A15B}">
+  <dimension ref="E5:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="46.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="5:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed section 3.3.Real World Federated Learning Settings.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA8331D0-D892-4FBA-8994-5C0E0FF5CE2D}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F629496A-FCE4-42F9-B459-1EBD29611DE3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t>FL</t>
   </si>
@@ -359,6 +359,18 @@
   </si>
   <si>
     <t>Trains models across multiple devices using Stochastic Gradient Descent, preserves centralized control, and reduces communication rounds.  It is efficient in non-IID data environments.</t>
+  </si>
+  <si>
+    <t>AML</t>
+  </si>
+  <si>
+    <t>Azure Machine Learning</t>
+  </si>
+  <si>
+    <t>JN</t>
+  </si>
+  <si>
+    <t>Jupyter Notebook</t>
   </si>
 </sst>
 </file>
@@ -507,6 +519,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -527,9 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,6 +1055,22 @@
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1812,28 +1840,28 @@
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
-      <c r="O15" s="17" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+      <c r="O15" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="17"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -2018,11 +2046,11 @@
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2039,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3C5ED9-A3DC-46C6-9548-9775EC56A15B}">
   <dimension ref="E5:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2090,7 +2118,7 @@
       </c>
     </row>
     <row r="14" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F14" s="21"/>
+      <c r="F14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed section, Federated Learning Datasets.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F629496A-FCE4-42F9-B459-1EBD29611DE3}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA3780C2-CC55-4F76-9571-55297CA9AE6D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="T.3.1." sheetId="3" r:id="rId3"/>
     <sheet name="T.3.2." sheetId="4" r:id="rId4"/>
     <sheet name="T.3.2.5." sheetId="5" r:id="rId5"/>
+    <sheet name="T.3.4." sheetId="6" r:id="rId6"/>
+    <sheet name="T.3.4.1." sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$K$4</definedName>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="154">
   <si>
     <t>FL</t>
   </si>
@@ -371,6 +373,141 @@
   </si>
   <si>
     <t>Jupyter Notebook</t>
+  </si>
+  <si>
+    <t>Datasets</t>
+  </si>
+  <si>
+    <t>Medical Imaging and Synthetic Datasets</t>
+  </si>
+  <si>
+    <t>Breast Cancer Wisconsin, Retail Transaction and Bank Marketing Datasets</t>
+  </si>
+  <si>
+    <t>MNIST, CIFAR-10 and MedNIST</t>
+  </si>
+  <si>
+    <t>CIFAR-10, Fashion-MNIST and IMDB</t>
+  </si>
+  <si>
+    <t>MNIST, CIFAR-10 and Shakespeare</t>
+  </si>
+  <si>
+    <t>EMNIST, CIFAR-10 and Shakespeare</t>
+  </si>
+  <si>
+    <t>LIDC-IDRI, BRATS and COVID-19 Chest X-ray</t>
+  </si>
+  <si>
+    <t>CIFAR-10, MNIST and ILSVRC2012</t>
+  </si>
+  <si>
+    <t>Medical  and Financial Datasets</t>
+  </si>
+  <si>
+    <t>Synthetic Data, CIFAR-10 and MNIST</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>MNIST</t>
+  </si>
+  <si>
+    <t>CIFAR-10</t>
+  </si>
+  <si>
+    <t>Used for image recognition tasks, providing a harder dataset to test the robustness of FL models. Used in Flower, FedML, and PaddleFL frameworks.</t>
+  </si>
+  <si>
+    <t>MedNIST</t>
+  </si>
+  <si>
+    <t>Applied in medical imaging for classification tasks, supporting healthcare applications with privacy-preserving capabilities. Used in PySyft.</t>
+  </si>
+  <si>
+    <t>EMNIST</t>
+  </si>
+  <si>
+    <t>An extension of MNIST for more extensive character recognition tasks. Used with TensorFlow Federated.</t>
+  </si>
+  <si>
+    <t>Fashion-MNIST</t>
+  </si>
+  <si>
+    <t>Focuses on recognizing fashion objects, providing a robust testing platform for machine-learning algorithms. Used in Flower.</t>
+  </si>
+  <si>
+    <t>IMDB</t>
+  </si>
+  <si>
+    <t>Used for sentiment analysis in natural language processing, providing a text-based dataset for FL models. Used in Flower.</t>
+  </si>
+  <si>
+    <t>Shakespeare</t>
+  </si>
+  <si>
+    <t>Medical Imaging Datasets (LIDC-IDRI, BRATS, COVID-19 Chest X-ray)</t>
+  </si>
+  <si>
+    <t>Retail Transaction and Bank Marketing Data</t>
+  </si>
+  <si>
+    <t>Used in financial services for fraud detection and predictive marketing. Discussed in FATE.</t>
+  </si>
+  <si>
+    <t>Synthetic Data</t>
+  </si>
+  <si>
+    <t>Commonly used in initial testing and benchmarking of FL algorithms before applying them to real datasets. Employed in FLGo.</t>
+  </si>
+  <si>
+    <t>Real-World Image Dataset by Luo et al. (2021)</t>
+  </si>
+  <si>
+    <t>A non-IID, imbalanced dataset from images recorded by 26 street cameras, classified into 7 object types. Evaluated with YOLO and Faster R-CNN in federated learning.</t>
+  </si>
+  <si>
+    <t>RSNA Chest X-ray Dataset</t>
+  </si>
+  <si>
+    <t>5,786 images for pneumonia detection, used to benchmark federated learning models across institutions while preserving data privacy. Described in Zhang, D. et al. (2021).</t>
+  </si>
+  <si>
+    <t>Keyword Spotting Datasets</t>
+  </si>
+  <si>
+    <t>Employed to model heterogeneity in non-IID conditions within federated learning for medical applications. Described in Pfitzer et al. (2021).</t>
+  </si>
+  <si>
+    <t>CIFAR-100</t>
+  </si>
+  <si>
+    <t>Effective in simulating non-IID conditions. Used in Lai et al. (2024).</t>
+  </si>
+  <si>
+    <t>Used for the classification of handwritten digits, providing an easy and effective benchmark for image classifications. Used by PySyft, FedML, and TFF.</t>
+  </si>
+  <si>
+    <t>Used for various medical tasks such as lung cancer screening, brain tumor segmentation, and COVID-19 detection. Used in NF and OpenFL.</t>
+  </si>
+  <si>
+    <t>Used for next-word prediction tasks in NLP, helping evaluate FL models in text prediction. Mentioned in FedML and TFF.</t>
+  </si>
+  <si>
+    <t>non-IID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-Independent and Identically Distributed </t>
+  </si>
+  <si>
+    <t>RSNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiological Society of North America </t>
   </si>
 </sst>
 </file>
@@ -480,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -543,6 +680,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,6 +705,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -877,16 +1028,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -899,183 +1050,199 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
-    <sortCondition ref="A2:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1160,7 +1327,7 @@
   <dimension ref="C4:W19"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="O4" sqref="O4:W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,7 +2081,7 @@
   <dimension ref="D3:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D14" sqref="D14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2068,7 +2235,7 @@
   <dimension ref="E5:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2123,4 +2290,323 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009A2148-9647-4EBA-9FD8-3280FD328B92}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.5546875" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="G2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="G3" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="G4" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="G5" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="G6" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="G7" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="G8" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="G9" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="G10" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="G11" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G12" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G13:I13"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I10" r:id="rId1" xr:uid="{FE27E248-B639-4DF6-9EEB-FD6AFD6EFF72}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637F5A8A-13AC-491D-B4D8-34EE3ECD90F1}">
+  <dimension ref="F3:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="123.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="6:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="6:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F17" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Literature review completed. Starting with Experimentation.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25DCD93C-3773-43E0-AA10-4EA5028C1024}"/>
+  <xr:revisionPtr revIDLastSave="379" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5BAA8F-66EF-4D02-84D4-E249B7A4672C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="7" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,11 @@
     <sheet name="T.3.2.5." sheetId="5" r:id="rId5"/>
     <sheet name="T.3.4." sheetId="6" r:id="rId6"/>
     <sheet name="T.3.4.1." sheetId="7" r:id="rId7"/>
+    <sheet name="T.3.6." sheetId="8" r:id="rId8"/>
+    <sheet name="T.3.6.1." sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$K$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
   </definedNames>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="174">
   <si>
     <t>FL</t>
   </si>
@@ -520,6 +523,54 @@
   </si>
   <si>
     <t xml:space="preserve">Representational State Transfer </t>
+  </si>
+  <si>
+    <t>RO(s)</t>
+  </si>
+  <si>
+    <t>Research Objective(s)</t>
+  </si>
+  <si>
+    <t>Literature Review</t>
+  </si>
+  <si>
+    <t>3.1. FL Frameworks</t>
+  </si>
+  <si>
+    <t>3.2. FL Algorithms</t>
+  </si>
+  <si>
+    <t>3.3. Real-World FL Settings</t>
+  </si>
+  <si>
+    <t>3.4. FL Datasets</t>
+  </si>
+  <si>
+    <t>3.5. FL Sever Implementation</t>
+  </si>
+  <si>
+    <t>To develop a FL Server</t>
+  </si>
+  <si>
+    <t>To Compare FL frameworks and the FL Server</t>
+  </si>
+  <si>
+    <t>To evaluate the implementatability of existing FL frameworks</t>
+  </si>
+  <si>
+    <t>Research Objectives</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>FL Frameworks: Sample (PySyft, FATE, Flower FedML and TensorFlow Federated)</t>
+  </si>
+  <si>
+    <t>FL Datasets: Sample (RSNA Chest X-ray, MNIST, and a synthetic data )</t>
+  </si>
+  <si>
+    <t>Clients: Sample (Medical and Technological)</t>
   </si>
 </sst>
 </file>
@@ -557,12 +608,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -629,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -701,6 +758,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:B27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,189 +1155,202 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>105</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>156</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>152</v>
+        <v>74</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>157</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B28" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B28">
+      <sortCondition ref="A2:A28"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B25">
     <sortCondition ref="A2:A25"/>
   </sortState>
@@ -2505,7 +2587,7 @@
   <dimension ref="F3:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,4 +2719,174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7AC6C-BAC7-4B34-9D95-C68F6FA49393}">
+  <dimension ref="E4:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
+    <col min="6" max="6" width="53.77734375" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="5:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+    </row>
+    <row r="9" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G5:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FCD28B-1E36-4558-8911-86FA7965D0F7}">
+  <dimension ref="F6:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="28.109375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G6" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" s="28"/>
+      <c r="I9" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G10" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I6:J6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding introduction, 5.Evaluating FL frameworks.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5BAA8F-66EF-4D02-84D4-E249B7A4672C}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AF57940-FAB4-419C-8E40-CD89F60CBBE3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="7" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="T.3.4.1." sheetId="7" r:id="rId7"/>
     <sheet name="T.3.6." sheetId="8" r:id="rId8"/>
     <sheet name="T.3.6.1." sheetId="10" r:id="rId9"/>
+    <sheet name="T.5" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="187">
   <si>
     <t>FL</t>
   </si>
@@ -571,6 +572,153 @@
   </si>
   <si>
     <t>Clients: Sample (Medical and Technological)</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>8-9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Poor:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The framework does not meet the requirements or performs very poorly.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Fair:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The framework meets the basic requirements but has significant limitations.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Good: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>The framework meets the requirements adequately but has some minor limitations.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Very Good:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The framework performs well and meets most requirements with minor issues.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Excellent:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The framework performs exceptionally well and meets all requirements with no significant issues.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Outstanding:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The framework exceeds expectations and offers superior performance and features.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -580,7 +728,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +754,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -686,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -738,6 +894,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -765,11 +924,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1358,6 +1520,87 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE450B4-7C85-4A17-990B-BEB82D7C7E18}">
+  <dimension ref="D4:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="52.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="30"/>
+      <c r="E4" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="31"/>
+      <c r="E5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D6" s="31"/>
+      <c r="E6" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="31"/>
+      <c r="E7" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D8" s="31"/>
+      <c r="E8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="31"/>
+      <c r="E9" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D10" s="31"/>
+      <c r="E10" s="4">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FC161B-4D55-42B8-B4B0-987B8811384D}">
   <dimension ref="D4:F8"/>
@@ -2117,28 +2360,28 @@
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
-      <c r="O15" s="22" t="s">
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
+      <c r="O15" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -2323,11 +2566,11 @@
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2565,11 +2808,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2725,7 +2968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7AC6C-BAC7-4B34-9D95-C68F6FA49393}">
   <dimension ref="E4:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
@@ -2740,19 +2983,19 @@
       <c r="E4" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="5:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="28" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2760,31 +3003,31 @@
       <c r="E6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E9" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2802,7 +3045,7 @@
   <dimension ref="F6:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2822,19 +3065,19 @@
       <c r="H6" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="J6" s="22"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="27" t="s">
         <v>168</v>
       </c>
       <c r="J7" s="29" t="s">
@@ -2845,16 +3088,16 @@
       <c r="G8" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="29"/>
     </row>
     <row r="9" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G9" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="26" t="s">
+      <c r="H9" s="19"/>
+      <c r="I9" s="27" t="s">
         <v>166</v>
       </c>
       <c r="J9" s="29"/>
@@ -2866,7 +3109,7 @@
       <c r="H10" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="I10" s="26"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="29"/>
     </row>
     <row r="11" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2876,7 +3119,7 @@
       <c r="H11" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="I11" s="26"/>
+      <c r="I11" s="27"/>
       <c r="J11" s="29"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FedML section completed. Word count 6,181 words left.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AF57940-FAB4-419C-8E40-CD89F60CBBE3}"/>
+  <xr:revisionPtr revIDLastSave="421" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDA3F96E-7027-4BE4-A731-A8543DAB5F37}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="189">
   <si>
     <t>FL</t>
   </si>
@@ -365,12 +365,6 @@
   </si>
   <si>
     <t>Azure Machine Learning</t>
-  </si>
-  <si>
-    <t>JN</t>
-  </si>
-  <si>
-    <t>Jupyter Notebook</t>
   </si>
   <si>
     <t>Datasets</t>
@@ -719,6 +713,18 @@
       </rPr>
       <t xml:space="preserve"> The framework exceeds expectations and offers superior performance and features.</t>
     </r>
+  </si>
+  <si>
+    <t>JN(s)</t>
+  </si>
+  <si>
+    <t>Jupyter Notebook(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUC </t>
+  </si>
+  <si>
+    <t>Area Under the Curve</t>
   </si>
 </sst>
 </file>
@@ -897,6 +903,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -926,12 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1271,15 +1277,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1301,209 +1307,217 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>105</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1513,8 +1527,8 @@
       <sortCondition ref="A2:A28"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B25">
-    <sortCondition ref="A2:A25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
+    <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1524,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE450B4-7C85-4A17-990B-BEB82D7C7E18}">
   <dimension ref="D4:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1534,66 +1548,66 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="30"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="21"/>
+      <c r="E5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D6" s="21"/>
+      <c r="E6" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D5" s="31"/>
-      <c r="E5" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="21"/>
+      <c r="E7" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D6" s="31"/>
-      <c r="E6" s="4" t="s">
+    <row r="8" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D8" s="21"/>
+      <c r="E8" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D7" s="31"/>
-      <c r="E7" s="4" t="s">
+    <row r="9" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="21"/>
+      <c r="E9" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D8" s="31"/>
-      <c r="E8" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D9" s="31"/>
-      <c r="E9" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
     <row r="10" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="31"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="4">
         <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2360,28 +2374,28 @@
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="22"/>
-      <c r="O15" s="23" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="24"/>
+      <c r="O15" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -2566,11 +2580,11 @@
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2670,7 +2684,7 @@
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="G2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>37</v>
@@ -2683,7 +2697,7 @@
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="G3" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>45</v>
@@ -2696,7 +2710,7 @@
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="G4" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>44</v>
@@ -2709,7 +2723,7 @@
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="G5" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>42</v>
@@ -2722,7 +2736,7 @@
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="G6" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>58</v>
@@ -2735,7 +2749,7 @@
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="G7" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>9</v>
@@ -2748,7 +2762,7 @@
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="G8" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>46</v>
@@ -2761,7 +2775,7 @@
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="G9" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>41</v>
@@ -2774,7 +2788,7 @@
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="G10" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>56</v>
@@ -2787,7 +2801,7 @@
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="G11" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>43</v>
@@ -2798,7 +2812,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G12" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>47</v>
@@ -2808,11 +2822,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2841,122 +2855,122 @@
   <sheetData>
     <row r="3" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F3" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F4" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F5" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F6" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F7" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F8" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F9" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F10" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="6:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F11" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F12" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F13" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="6:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F14" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F15" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F16" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2981,53 +2995,53 @@
   <sheetData>
     <row r="4" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="23"/>
+        <v>158</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="5:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E6" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+        <v>160</v>
+      </c>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="28"/>
+        <v>161</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+        <v>162</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E9" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
+        <v>163</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3060,67 +3074,67 @@
   <sheetData>
     <row r="6" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G6" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="J6" s="23"/>
+        <v>168</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G7" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G8" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="29"/>
+        <v>160</v>
+      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="31"/>
     </row>
     <row r="9" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G9" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H9" s="19"/>
-      <c r="I9" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="J9" s="29"/>
+      <c r="I9" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G10" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="29"/>
+        <v>170</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="31"/>
     </row>
     <row r="11" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G11" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="29"/>
+        <v>171</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
TensorFlow Federated section completed.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDA3F96E-7027-4BE4-A731-A8543DAB5F37}"/>
+  <xr:revisionPtr revIDLastSave="424" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E23D53B1-08B7-4093-A59A-6788DD0FEB74}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="190">
   <si>
     <t>FL</t>
   </si>
@@ -725,6 +725,9 @@
   </si>
   <si>
     <t>Area Under the Curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC </t>
   </si>
 </sst>
 </file>
@@ -1277,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B29"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,153 +1374,161 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>185</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>91</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1527,8 +1538,8 @@
       <sortCondition ref="A2:A28"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
-    <sortCondition ref="A2:A29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B30">
+    <sortCondition ref="A2:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2524,7 +2535,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D9" s="13" t="s">
         <v>85</v>
       </c>
@@ -2568,7 +2579,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Evaluation FL frameworks completed.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E23D53B1-08B7-4093-A59A-6788DD0FEB74}"/>
+  <xr:revisionPtr revIDLastSave="477" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{165E08B3-D8F9-4EC5-8EED-F8A2A4EC73BF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="10" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="T.3.6." sheetId="8" r:id="rId8"/>
     <sheet name="T.3.6.1." sheetId="10" r:id="rId9"/>
     <sheet name="T.5" sheetId="11" r:id="rId10"/>
+    <sheet name="T.6" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="206">
   <si>
     <t>FL</t>
   </si>
@@ -728,6 +729,54 @@
   </si>
   <si>
     <t xml:space="preserve">FC </t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Setup and Configuration</t>
+  </si>
+  <si>
+    <t>Examples and Tutorials</t>
+  </si>
+  <si>
+    <t>Custom Algorithm Implementation</t>
+  </si>
+  <si>
+    <t>Adaptability to Various Use Cases</t>
+  </si>
+  <si>
+    <t>Industry Adoption</t>
+  </si>
+  <si>
+    <t>Average Score</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>Ease of use</t>
+  </si>
+  <si>
+    <t>Flexibility and customisability</t>
+  </si>
+  <si>
+    <t>Real-world applicability</t>
   </si>
 </sst>
 </file>
@@ -787,7 +836,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -847,11 +896,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -941,6 +1010,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1282,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,7 +1625,7 @@
   <dimension ref="D4:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,6 +1697,204 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251AAA7B-FC40-4F27-8AA6-A9DBE55EA49F}">
+  <dimension ref="D4:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D6" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="12">
+        <v>8</v>
+      </c>
+      <c r="G6" s="12">
+        <v>8</v>
+      </c>
+      <c r="H6" s="12">
+        <v>7</v>
+      </c>
+      <c r="I6" s="12">
+        <v>8</v>
+      </c>
+      <c r="J6" s="12">
+        <v>7</v>
+      </c>
+      <c r="K6" s="4">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="12">
+        <v>7</v>
+      </c>
+      <c r="G7" s="12">
+        <v>8</v>
+      </c>
+      <c r="H7" s="12">
+        <v>8</v>
+      </c>
+      <c r="I7" s="12">
+        <v>8</v>
+      </c>
+      <c r="J7" s="12">
+        <v>6</v>
+      </c>
+      <c r="K7" s="4">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D8" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="12">
+        <v>6</v>
+      </c>
+      <c r="G8" s="12">
+        <v>7</v>
+      </c>
+      <c r="H8" s="12">
+        <v>9</v>
+      </c>
+      <c r="I8" s="12">
+        <v>7</v>
+      </c>
+      <c r="J8" s="12">
+        <v>7</v>
+      </c>
+      <c r="K8" s="4">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="12">
+        <v>6</v>
+      </c>
+      <c r="G9" s="12">
+        <v>6</v>
+      </c>
+      <c r="H9" s="12">
+        <v>7</v>
+      </c>
+      <c r="I9" s="12">
+        <v>6</v>
+      </c>
+      <c r="J9" s="12">
+        <v>6</v>
+      </c>
+      <c r="K9" s="4">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="12">
+        <v>5</v>
+      </c>
+      <c r="G10" s="12">
+        <v>5</v>
+      </c>
+      <c r="H10" s="12">
+        <v>6</v>
+      </c>
+      <c r="I10" s="12">
+        <v>5</v>
+      </c>
+      <c r="J10" s="12">
+        <v>4</v>
+      </c>
+      <c r="K10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updating score criteria for FL frameworks.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="477" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{165E08B3-D8F9-4EC5-8EED-F8A2A4EC73BF}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A38E6E-EE02-4C1E-8930-05973C92AC44}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="10" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="T.3.6.1." sheetId="10" r:id="rId9"/>
     <sheet name="T.5" sheetId="11" r:id="rId10"/>
     <sheet name="T.6" sheetId="12" r:id="rId11"/>
+    <sheet name="T.6 (2)" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="216">
   <si>
     <t>FL</t>
   </si>
@@ -777,6 +778,36 @@
   </si>
   <si>
     <t>Real-world applicability</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>FedML AI Inc.</t>
+  </si>
+  <si>
+    <t>Adap GmbH</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>WeBank &amp; Linux Foundation</t>
+  </si>
+  <si>
+    <t>OpenMined</t>
+  </si>
+  <si>
+    <t>Look and see what other people have done. To evaluate FL frameworks. Look if there is an standard. Explain why did you picked. Also look at weights.</t>
+  </si>
+  <si>
+    <t>Close to Real-world Settings??</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Setup and Configuration</t>
   </si>
 </sst>
 </file>
@@ -920,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1017,6 +1048,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,10 +1083,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1703,37 +1750,42 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251AAA7B-FC40-4F27-8AA6-A9DBE55EA49F}">
-  <dimension ref="D4:K10"/>
+  <dimension ref="D4:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="5" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="130.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="25"/>
+      <c r="K4" s="4" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O4" s="34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="4:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D5" s="4" t="s">
         <v>190</v>
       </c>
@@ -1741,159 +1793,570 @@
         <v>191</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D6" s="12" t="s">
         <v>198</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="12">
-        <v>8</v>
+      <c r="F6" s="35" t="s">
+        <v>207</v>
       </c>
       <c r="G6" s="12">
         <v>8</v>
       </c>
       <c r="H6" s="12">
+        <v>8</v>
+      </c>
+      <c r="I6" s="12">
         <v>7</v>
+      </c>
+      <c r="J6" s="12">
+        <v>8</v>
+      </c>
+      <c r="K6" s="12">
+        <v>7</v>
+      </c>
+      <c r="L6" s="4">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="12">
+        <v>7</v>
+      </c>
+      <c r="H7" s="12">
+        <v>8</v>
+      </c>
+      <c r="I7" s="12">
+        <v>8</v>
+      </c>
+      <c r="J7" s="12">
+        <v>8</v>
+      </c>
+      <c r="K7" s="12">
+        <v>6</v>
+      </c>
+      <c r="L7" s="4">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D8" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="G8" s="12">
+        <v>6</v>
+      </c>
+      <c r="H8" s="12">
+        <v>7</v>
+      </c>
+      <c r="I8" s="12">
+        <v>7</v>
+      </c>
+      <c r="J8" s="12">
+        <v>7</v>
+      </c>
+      <c r="K8" s="12">
+        <v>7</v>
+      </c>
+      <c r="L8" s="4">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="9" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D9" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="12">
+        <v>6</v>
+      </c>
+      <c r="H9" s="12">
+        <v>6</v>
+      </c>
+      <c r="I9" s="12">
+        <v>9</v>
+      </c>
+      <c r="J9" s="12">
+        <v>6</v>
+      </c>
+      <c r="K9" s="12">
+        <v>6</v>
+      </c>
+      <c r="L9" s="4">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D10" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="12">
+        <v>5</v>
+      </c>
+      <c r="H10" s="12">
+        <v>5</v>
+      </c>
+      <c r="I10" s="12">
+        <v>6</v>
+      </c>
+      <c r="J10" s="12">
+        <v>5</v>
+      </c>
+      <c r="K10" s="12">
+        <v>4</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="D4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E6934E-D7C4-484C-AEBC-9F58A7487085}">
+  <dimension ref="D4:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.44140625" customWidth="1"/>
+    <col min="14" max="14" width="130.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="N4" s="34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D6" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="12">
+        <v>7</v>
+      </c>
+      <c r="H6" s="12">
+        <v>8</v>
       </c>
       <c r="I6" s="12">
         <v>8</v>
       </c>
-      <c r="J6" s="12">
-        <v>7</v>
-      </c>
-      <c r="K6" s="4">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="J6" s="41">
+        <f>SUM(G6:I6)/3</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="K6" s="40"/>
+    </row>
+    <row r="7" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D7" s="12" t="s">
         <v>199</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="12">
         <v>7</v>
-      </c>
-      <c r="G7" s="12">
-        <v>8</v>
       </c>
       <c r="H7" s="12">
         <v>8</v>
       </c>
       <c r="I7" s="12">
-        <v>8</v>
-      </c>
-      <c r="J7" s="12">
-        <v>6</v>
-      </c>
-      <c r="K7" s="4">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="J7" s="41">
+        <f t="shared" ref="J7:J10" si="0">SUM(G7:I7)/3</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="K7" s="40"/>
+    </row>
+    <row r="8" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="12" t="s">
         <v>200</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="12">
+        <v>44</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="G8" s="12">
         <v>6</v>
       </c>
-      <c r="G8" s="12">
+      <c r="H8" s="12">
         <v>7</v>
-      </c>
-      <c r="H8" s="12">
-        <v>9</v>
       </c>
       <c r="I8" s="12">
         <v>7</v>
       </c>
-      <c r="J8" s="12">
-        <v>7</v>
-      </c>
-      <c r="K8" s="4">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="J8" s="41">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="K8" s="40"/>
+    </row>
+    <row r="9" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D9" s="12" t="s">
         <v>201</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="12">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="12">
+        <v>7</v>
+      </c>
+      <c r="H9" s="12">
         <v>6</v>
-      </c>
-      <c r="G9" s="12">
-        <v>6</v>
-      </c>
-      <c r="H9" s="12">
-        <v>7</v>
       </c>
       <c r="I9" s="12">
         <v>6</v>
       </c>
-      <c r="J9" s="12">
-        <v>6</v>
-      </c>
-      <c r="K9" s="4">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="J9" s="41">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="K9" s="40"/>
+    </row>
+    <row r="10" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D10" s="12" t="s">
         <v>202</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="12">
-        <v>5</v>
+      <c r="F10" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="G10" s="12">
         <v>5</v>
       </c>
       <c r="H10" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10" s="12">
         <v>5</v>
       </c>
-      <c r="J10" s="12">
-        <v>4</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="J10" s="41">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="K10" s="40"/>
+    </row>
+    <row r="13" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+    </row>
+    <row r="14" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
+  <mergeCells count="2">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting with section 6.Federated Learning Server Development. 5,538 words left.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="546" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A38E6E-EE02-4C1E-8930-05973C92AC44}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21DD318-6476-4AF7-AA14-CB159634718E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="215">
   <si>
     <t>FL</t>
   </si>
@@ -799,9 +799,6 @@
   </si>
   <si>
     <t>Look and see what other people have done. To evaluate FL frameworks. Look if there is an standard. Explain why did you picked. Also look at weights.</t>
-  </si>
-  <si>
-    <t>Close to Real-world Settings??</t>
   </si>
   <si>
     <t>Average</t>
@@ -951,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1012,6 +1009,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1048,26 +1061,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,6 +1076,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1750,7 +1747,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251AAA7B-FC40-4F27-8AA6-A9DBE55EA49F}">
-  <dimension ref="D4:O20"/>
+  <dimension ref="D4:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:L10"/>
@@ -1767,21 +1764,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="25" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="31"/>
+      <c r="I4" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="24" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1821,7 +1818,7 @@
       <c r="E6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="22" t="s">
         <v>207</v>
       </c>
       <c r="G6" s="12">
@@ -1850,7 +1847,7 @@
       <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="22" t="s">
         <v>208</v>
       </c>
       <c r="G7" s="12">
@@ -1879,7 +1876,7 @@
       <c r="E8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="23" t="s">
         <v>210</v>
       </c>
       <c r="G8" s="12">
@@ -1937,7 +1934,7 @@
       <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="22" t="s">
         <v>211</v>
       </c>
       <c r="G10" s="12">
@@ -1959,109 +1956,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-    </row>
     <row r="14" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-    </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-    </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="15"/>
+      <c r="F17" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2075,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E6934E-D7C4-484C-AEBC-9F58A7487085}">
-  <dimension ref="D4:N20"/>
+  <dimension ref="D4:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,19 +1999,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="25" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="25"/>
+      <c r="H4" s="31"/>
       <c r="I4" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="N4" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="N4" s="24" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2119,7 +2026,7 @@
         <v>206</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>195</v>
@@ -2128,9 +2035,9 @@
         <v>193</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K5" s="38"/>
+        <v>213</v>
+      </c>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D6" s="12" t="s">
@@ -2139,7 +2046,7 @@
       <c r="E6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="22" t="s">
         <v>207</v>
       </c>
       <c r="G6" s="12">
@@ -2151,11 +2058,11 @@
       <c r="I6" s="12">
         <v>8</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="27">
         <f>SUM(G6:I6)/3</f>
         <v>7.666666666666667</v>
       </c>
-      <c r="K6" s="40"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D7" s="12" t="s">
@@ -2164,7 +2071,7 @@
       <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="22" t="s">
         <v>208</v>
       </c>
       <c r="G7" s="12">
@@ -2176,11 +2083,11 @@
       <c r="I7" s="12">
         <v>7</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="27">
         <f t="shared" ref="J7:J10" si="0">SUM(G7:I7)/3</f>
         <v>7.333333333333333</v>
       </c>
-      <c r="K7" s="40"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="12" t="s">
@@ -2189,7 +2096,7 @@
       <c r="E8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="23" t="s">
         <v>210</v>
       </c>
       <c r="G8" s="12">
@@ -2201,11 +2108,11 @@
       <c r="I8" s="12">
         <v>7</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="27">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
-      <c r="K8" s="40"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D9" s="12" t="s">
@@ -2226,11 +2133,11 @@
       <c r="I9" s="12">
         <v>6</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="27">
         <f t="shared" si="0"/>
         <v>6.333333333333333</v>
       </c>
-      <c r="K9" s="40"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D10" s="12" t="s">
@@ -2239,7 +2146,7 @@
       <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="22" t="s">
         <v>211</v>
       </c>
       <c r="G10" s="12">
@@ -2251,107 +2158,24 @@
       <c r="I10" s="12">
         <v>5</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="27">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K10" s="40"/>
-    </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-    </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-    </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-    </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="15"/>
+      <c r="F17" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3121,28 +2945,28 @@
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
-      <c r="O15" s="25" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="O15" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -3327,11 +3151,11 @@
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3569,11 +3393,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3744,19 +3568,19 @@
       <c r="E4" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="5:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="36" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3764,31 +3588,31 @@
       <c r="E6" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E9" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3826,22 +3650,22 @@
       <c r="H6" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="37" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3849,19 +3673,19 @@
       <c r="G8" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="31"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G9" s="4" t="s">
         <v>161</v>
       </c>
       <c r="H9" s="19"/>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="J9" s="31"/>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G10" s="4" t="s">
@@ -3870,8 +3694,8 @@
       <c r="H10" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="31"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G11" s="4" t="s">
@@ -3880,8 +3704,8 @@
       <c r="H11" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="31"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
FL Server report 481 word count section. Words left total word count 5,093. Next section communication protocols.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21DD318-6476-4AF7-AA14-CB159634718E}"/>
+  <xr:revisionPtr revIDLastSave="814" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9A3E015-5D20-4162-A108-EB9E490748D9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="715" firstSheet="7" activeTab="15" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,11 @@
     <sheet name="T.5" sheetId="11" r:id="rId10"/>
     <sheet name="T.6" sheetId="12" r:id="rId11"/>
     <sheet name="T.6 (2)" sheetId="13" r:id="rId12"/>
+    <sheet name="Table 6.2.1" sheetId="16" r:id="rId13"/>
+    <sheet name="T.Server.py" sheetId="14" r:id="rId14"/>
+    <sheet name="T.Client.py" sheetId="15" r:id="rId15"/>
+    <sheet name="Table 6.2.2" sheetId="17" r:id="rId16"/>
+    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
@@ -52,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="363">
   <si>
     <t>FL</t>
   </si>
@@ -806,6 +811,664 @@
   <si>
     <t xml:space="preserve"> Setup and Configuration</t>
   </si>
+  <si>
+    <t>def aggregate_models(client_updates):</t>
+  </si>
+  <si>
+    <t>Aggregates the model weights received from all clients by averaging them. Also aggregates and updates metrics across all rounds. After aggregation, it resets client statuses to 'ready' and triggers a server refresh.</t>
+  </si>
+  <si>
+    <t>def index():</t>
+  </si>
+  <si>
+    <t>Renders the main dashboard page of the FL server, displaying the status and metrics of all registered clients as well as the global model metrics.</t>
+  </si>
+  <si>
+    <t>def register_client():</t>
+  </si>
+  <si>
+    <t>Registers a client with the server by recording its client ID, port, and host address. Updates the server when a certain number of clients are registered and triggers a refresh.</t>
+  </si>
+  <si>
+    <t>def client_ready():</t>
+  </si>
+  <si>
+    <t>Updates the server when a client is ready to start training. It sets the client's status to 'ready' and logs the client's readiness.</t>
+  </si>
+  <si>
+    <t>def update_model():</t>
+  </si>
+  <si>
+    <t>Receives model updates from clients, including the model weights and training metrics. Aggregates models and sends the updated global model back to all clients once all clients have completed their updates. Triggers a refresh after aggregation.</t>
+  </si>
+  <si>
+    <t>def start_training():</t>
+  </si>
+  <si>
+    <t>Starts a training session for a specified dataset. Sends a command to all clients to prepare for training. Uses threading to wait until all clients are ready before starting the training.</t>
+  </si>
+  <si>
+    <t>def prepare_training():</t>
+  </si>
+  <si>
+    <t>Prepares the server-side setup for a client to train on a specified dataset. Marks the client as ready once the preparation is complete.</t>
+  </si>
+  <si>
+    <t>def wait_and_start_clients(dataset):</t>
+  </si>
+  <si>
+    <t>A helper function that waits for all clients to be ready before sending the start training signal to each client. Ensures that training only begins when all clients are synchronized.</t>
+  </si>
+  <si>
+    <t>def update_client_status():</t>
+  </si>
+  <si>
+    <t>Updates the status of a client on the server (e.g., ready, training, etc.) based on the information sent by the client.</t>
+  </si>
+  <si>
+    <t>def debug_clients():</t>
+  </si>
+  <si>
+    <t>Provides a debug endpoint that returns the current state of all registered clients in JSON format, useful for debugging and monitoring the server's state.</t>
+  </si>
+  <si>
+    <t>def set_refresh():</t>
+  </si>
+  <si>
+    <t>def clear_refresh():</t>
+  </si>
+  <si>
+    <t>def should_refresh():</t>
+  </si>
+  <si>
+    <t>def reset():</t>
+  </si>
+  <si>
+    <t>Resets the server state, including the global model, metrics, and client statuses. Notifies all clients to reset as well and triggers a server refresh.</t>
+  </si>
+  <si>
+    <t>def shutdown():</t>
+  </si>
+  <si>
+    <t>Waits until all clients are ready before initiating the training process. This function ensures synchronization across clients, preventing any client from starting too early.</t>
+  </si>
+  <si>
+    <t>def app.run(debug=True, port=5000):</t>
+  </si>
+  <si>
+    <t>def load_data(client_id, scenario):</t>
+  </si>
+  <si>
+    <t>Loads and preprocesses the dataset for a given client and scenario. Supports both IID and non-IID data for technological scenarios. Returns split training and validation sets.</t>
+  </si>
+  <si>
+    <t>def load_medical_data_iid(client_id):</t>
+  </si>
+  <si>
+    <t>def load_medical_data_non_iid(client_id):</t>
+  </si>
+  <si>
+    <t>def create_simple_model(dataset):</t>
+  </si>
+  <si>
+    <t>Creates and returns a simple model architecture based on the dataset type (technological or medical). Uses sequential layers, including dense layers for technological datasets and convolutional layers for medical datasets.</t>
+  </si>
+  <si>
+    <t>Prepares the client for training by loading the appropriate dataset, creating the model, and compiling it. Sets the client's status to ready once preparation is complete.</t>
+  </si>
+  <si>
+    <t>Initiates the training process on the client upon receiving the command from the server. Starts a new training thread after verifying that the client is ready. Updates the server with the client’s status.</t>
+  </si>
+  <si>
+    <t>def run_training(dataset):</t>
+  </si>
+  <si>
+    <t>Performs the actual model training based on the loaded dataset. After training, it sends the updated model weights and metrics back to the server. It also handles any exceptions that occur during training and ensures the training status is properly managed.</t>
+  </si>
+  <si>
+    <t>def compile_model(dataset):</t>
+  </si>
+  <si>
+    <t>Compiles the model with an appropriate loss function and optimizer based on the dataset type. Ensures the model is ready for training.</t>
+  </si>
+  <si>
+    <t>def send_update(model, client_id, server_url, metrics, round_counter):</t>
+  </si>
+  <si>
+    <t>Sends the updated model weights and training metrics to the server after a training round is completed.</t>
+  </si>
+  <si>
+    <t>def receive_model():</t>
+  </si>
+  <si>
+    <t>Receives the global model weights from the server, updates the local model, and prepares the client for the next round of training. Logs the reception of the model and updates the client's status.</t>
+  </si>
+  <si>
+    <t>def reset_client():</t>
+  </si>
+  <si>
+    <t>Resets the client’s state, including reloading the dataset, resetting the round counter, and re-registering the client with the server. Ensures the client is ready for the next round of training after a reset.</t>
+  </si>
+  <si>
+    <t>Handles the shutdown command sent by the server, triggering the client to stop its operations.</t>
+  </si>
+  <si>
+    <t>def shutdown_server():</t>
+  </si>
+  <si>
+    <t>Forcefully stops the Flask server running the client, ensuring that the client process is terminated immediately.</t>
+  </si>
+  <si>
+    <t>def app.run(debug=True, host=args.host, port=args.port):</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sets the global </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>should_refresh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> flag to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, indicating that a page refresh is needed to reflect the latest server state.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Resets the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>should_refresh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> flag to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> after a refresh has been triggered, ensuring that the refresh state is only active when needed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Provides an endpoint that checks if the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>should_refresh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> flag is set. If so, it returns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and resets the flag, prompting a page refresh on the client-side.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notifies all connected clients that the server is shutting down and then gracefully stops the server. It uses </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>os._exit(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to immediately stop the server, ensuring no lingering processes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Runs the Flask application, initializing the server on port 5000. The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>debug=True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> option is set for development purposes, allowing for easier debugging and automatic reloading during development.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Loads IID medical image data for a specified client, preparing it for training using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ImageDataGenerator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Returns training and testing data generators.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Loads non-IID medical image data for a specified client, similar to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>load_medical_data_iid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, but for non-IID scenarios. Returns training and testing data generators.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Starts the Flask application, initializing the client on the specified host and port. The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>debug=True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> option is set for development purposes, allowing for easier debugging and automatic reloading during development.</t>
+    </r>
+  </si>
+  <si>
+    <t>Functions client.py</t>
+  </si>
+  <si>
+    <t>Functions server.py</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>HTTP Method</t>
+  </si>
+  <si>
+    <t>server.py</t>
+  </si>
+  <si>
+    <t>client.py</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Clients register themselves with the server by sending their ID, port, and host details.</t>
+  </si>
+  <si>
+    <t>Registers the client and updates server state.</t>
+  </si>
+  <si>
+    <t>Sends client details to the server for registration.</t>
+  </si>
+  <si>
+    <t>/client_ready</t>
+  </si>
+  <si>
+    <t>Clients notify the server that they are ready to begin training.</t>
+  </si>
+  <si>
+    <t>Updates client status to 'ready'.</t>
+  </si>
+  <si>
+    <t>Sends readiness status to the server.</t>
+  </si>
+  <si>
+    <t>/update</t>
+  </si>
+  <si>
+    <t>Clients send their model updates (weights and metrics) to the server after a training round.</t>
+  </si>
+  <si>
+    <t>Receives model updates and aggregates them.</t>
+  </si>
+  <si>
+    <t>Sends updated model weights and metrics to the server.</t>
+  </si>
+  <si>
+    <t>/start_training</t>
+  </si>
+  <si>
+    <t>The server sends a command to all clients to start the training process for a specific dataset.</t>
+  </si>
+  <si>
+    <t>Initiates training for all clients.</t>
+  </si>
+  <si>
+    <t>Receives start command and begins local training.</t>
+  </si>
+  <si>
+    <t>/prepare_training</t>
+  </si>
+  <si>
+    <t>The server instructs a specific client to prepare for training with a designated dataset.</t>
+  </si>
+  <si>
+    <t>Sends preparation command to specific client.</t>
+  </si>
+  <si>
+    <t>Prepares client for training based on the received dataset.</t>
+  </si>
+  <si>
+    <t>/client_status</t>
+  </si>
+  <si>
+    <t>Updates the status of a client on the server (e.g., ready, training).</t>
+  </si>
+  <si>
+    <t>Updates the status of a specific client.</t>
+  </si>
+  <si>
+    <t>Sends the current client status to the server.</t>
+  </si>
+  <si>
+    <t>/should_refresh</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Clients check whether they need to refresh their state based on server-side changes.</t>
+  </si>
+  <si>
+    <t>Indicates whether a refresh is required.</t>
+  </si>
+  <si>
+    <t>/reset_server</t>
+  </si>
+  <si>
+    <t>Resets the server's state, including the global model, metrics, and client statuses.</t>
+  </si>
+  <si>
+    <t>Resets server and notifies clients.</t>
+  </si>
+  <si>
+    <t>/shutdown</t>
+  </si>
+  <si>
+    <t>The server sends a shutdown command to all connected clients, then stops itself.</t>
+  </si>
+  <si>
+    <t>Shuts down the server and notifies clients.</t>
+  </si>
+  <si>
+    <t>Receives shutdown command and stops client operations.</t>
+  </si>
+  <si>
+    <t>/debug/clients</t>
+  </si>
+  <si>
+    <t>Provides a debug endpoint that returns the current state of all registered clients.</t>
+  </si>
+  <si>
+    <t>Returns the current state of all clients.</t>
+  </si>
+  <si>
+    <t>/receive_model</t>
+  </si>
+  <si>
+    <t>Receives the global model weights from the server and updates the local model.</t>
+  </si>
+  <si>
+    <t>Sends updated global model weights to clients.</t>
+  </si>
+  <si>
+    <t>Receives updated global model weights from the server.</t>
+  </si>
+  <si>
+    <t>/reset</t>
+  </si>
+  <si>
+    <t>Resets the client’s state and prepares it for the next round of training.</t>
+  </si>
+  <si>
+    <t>Sends reset command to clients.</t>
+  </si>
+  <si>
+    <t>Resets the client state and re-registers with the server</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML </t>
+  </si>
+  <si>
+    <t>Hypertext Markup Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESTful API </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON </t>
+  </si>
+  <si>
+    <t>Hypertext Transfer Protocol</t>
+  </si>
+  <si>
+    <t>Representational State Transfer Application Programming Interface</t>
+  </si>
+  <si>
+    <t>JavaScript Object Notation</t>
+  </si>
+  <si>
+    <t>register_client():</t>
+  </si>
+  <si>
+    <t>client_ready():</t>
+  </si>
+  <si>
+    <t>prepare_training():</t>
+  </si>
+  <si>
+    <t>update_model():</t>
+  </si>
+  <si>
+    <t>aggregate_models(client_updates):</t>
+  </si>
+  <si>
+    <t>index():</t>
+  </si>
+  <si>
+    <t>start_training():</t>
+  </si>
+  <si>
+    <t>wait_and_start_clients(dataset):</t>
+  </si>
+  <si>
+    <t>set_refresh():</t>
+  </si>
+  <si>
+    <t>clear_refresh():</t>
+  </si>
+  <si>
+    <t>should_refresh():</t>
+  </si>
+  <si>
+    <t>reset():</t>
+  </si>
+  <si>
+    <t>shutdown():</t>
+  </si>
+  <si>
+    <t>debug_clients():</t>
+  </si>
+  <si>
+    <t>update_client_status():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> load_data(client_id, scenario):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> load_medical_data_iid(client_id):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> load_medical_data_non_iid(client_id):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> create_simple_model(dataset):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prepare_training():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> start_training():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> run_training(dataset):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> compile_model(dataset):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> send_update(model, client_id, server_url, metrics, round_counter):</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> receive_model():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reset_client():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shutdown():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shutdown_server():</t>
+  </si>
 </sst>
 </file>
 
@@ -814,7 +1477,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +1511,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -948,7 +1617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1025,6 +1694,12 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1061,6 +1736,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,16 +2082,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1549,112 +2232,144 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>327</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>185</v>
+        <v>329</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>186</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>185</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>331</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>146</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>147</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>154</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>330</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B28" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B28">
-      <sortCondition ref="A2:A28"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B34">
+      <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B30">
@@ -1750,7 +2465,7 @@
   <dimension ref="D4:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:L10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,17 +2479,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="31" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31" t="s">
+      <c r="H4" s="33"/>
+      <c r="I4" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="31"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="4" t="s">
         <v>205</v>
       </c>
@@ -1984,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E6934E-D7C4-484C-AEBC-9F58A7487085}">
   <dimension ref="D4:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1999,13 +2714,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="31" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="31"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="4" t="s">
         <v>205</v>
       </c>
@@ -2182,6 +2897,754 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:H4"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D28749-D765-415A-9C12-E1FE75AF4B71}">
+  <dimension ref="C3:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="45" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" style="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="43"/>
+      <c r="F3" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="44"/>
+      <c r="F4" s="29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="44"/>
+      <c r="F5" s="29" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="44"/>
+      <c r="F6" s="29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="44"/>
+      <c r="F7" s="29" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="44"/>
+      <c r="F8" s="29" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="44"/>
+      <c r="F9" s="29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="44"/>
+      <c r="F10" s="29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="44"/>
+      <c r="F11" s="29" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="44"/>
+      <c r="F12" s="29" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="44"/>
+      <c r="F13" s="29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="44"/>
+      <c r="F14" s="29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="44"/>
+      <c r="F17" s="29" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="44"/>
+      <c r="F18" s="29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE30FFEC-DD3A-43C2-9692-82381583DFB4}">
+  <dimension ref="C3:D20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C5" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C6" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C9" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C12" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C13" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C14" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C16" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C17" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C18" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C19" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1877F309-2AC0-4525-B1B7-2FED63E9E5D6}">
+  <dimension ref="C3:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C5" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C6" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="C7" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="C10" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C12" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C16" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="C17" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D455F8B2-ECEE-4F97-AE0E-F30B6212FF7D}">
+  <dimension ref="C3:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="55.21875" customWidth="1"/>
+    <col min="5" max="5" width="55.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="29" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="29" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="29" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="29" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="29" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="29" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="29" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="29" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="29" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="29" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="29" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
+  <dimension ref="C3:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C4" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C7" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C8" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C9" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C11" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C12" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C13" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C14" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2945,28 +4408,28 @@
       </c>
     </row>
     <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="O15" s="31" t="s">
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+      <c r="O15" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -3151,11 +4614,11 @@
       </c>
     </row>
     <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3393,11 +4856,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3415,7 +4878,7 @@
   <dimension ref="F3:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3554,7 +5017,7 @@
   <dimension ref="E4:G9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3568,19 +5031,19 @@
       <c r="E4" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="31"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="5:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="38" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3588,31 +5051,31 @@
       <c r="E6" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E9" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3650,22 +5113,22 @@
       <c r="H6" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="31"/>
+      <c r="J6" s="33"/>
     </row>
     <row r="7" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="39" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3673,19 +5136,19 @@
       <c r="G8" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G9" s="4" t="s">
         <v>161</v>
       </c>
       <c r="H9" s="19"/>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="J9" s="37"/>
+      <c r="J9" s="39"/>
     </row>
     <row r="10" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G10" s="4" t="s">
@@ -3694,8 +5157,8 @@
       <c r="H10" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="39"/>
     </row>
     <row r="11" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G11" s="4" t="s">
@@ -3704,8 +5167,8 @@
       <c r="H11" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Completing section 6.4. Machine Learning Models Used. 4944 Words left.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="814" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9A3E015-5D20-4162-A108-EB9E490748D9}"/>
+  <xr:revisionPtr revIDLastSave="973" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA11D1B-AD06-4CB3-A576-9B93B7555E69}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="715" firstSheet="7" activeTab="15" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="48990" yWindow="150" windowWidth="17280" windowHeight="22770" tabRatio="715" firstSheet="12" activeTab="16" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,14 @@
     <sheet name="T.6 (2)" sheetId="13" r:id="rId12"/>
     <sheet name="Table 6.2.1" sheetId="16" r:id="rId13"/>
     <sheet name="T.Server.py" sheetId="14" r:id="rId14"/>
-    <sheet name="T.Client.py" sheetId="15" r:id="rId15"/>
-    <sheet name="Table 6.2.2" sheetId="17" r:id="rId16"/>
-    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId17"/>
+    <sheet name="Table 6.2.2" sheetId="17" r:id="rId15"/>
+    <sheet name="T.Client.py" sheetId="15" r:id="rId16"/>
+    <sheet name="Table 6.3. Endpoints and HTTP" sheetId="20" r:id="rId17"/>
+    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$K$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
   </definedNames>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="331">
   <si>
     <t>FL</t>
   </si>
@@ -812,105 +814,9 @@
     <t xml:space="preserve"> Setup and Configuration</t>
   </si>
   <si>
-    <t>def aggregate_models(client_updates):</t>
-  </si>
-  <si>
-    <t>Aggregates the model weights received from all clients by averaging them. Also aggregates and updates metrics across all rounds. After aggregation, it resets client statuses to 'ready' and triggers a server refresh.</t>
-  </si>
-  <si>
-    <t>def index():</t>
-  </si>
-  <si>
-    <t>Renders the main dashboard page of the FL server, displaying the status and metrics of all registered clients as well as the global model metrics.</t>
-  </si>
-  <si>
-    <t>def register_client():</t>
-  </si>
-  <si>
-    <t>Registers a client with the server by recording its client ID, port, and host address. Updates the server when a certain number of clients are registered and triggers a refresh.</t>
-  </si>
-  <si>
-    <t>def client_ready():</t>
-  </si>
-  <si>
-    <t>Updates the server when a client is ready to start training. It sets the client's status to 'ready' and logs the client's readiness.</t>
-  </si>
-  <si>
-    <t>def update_model():</t>
-  </si>
-  <si>
-    <t>Receives model updates from clients, including the model weights and training metrics. Aggregates models and sends the updated global model back to all clients once all clients have completed their updates. Triggers a refresh after aggregation.</t>
-  </si>
-  <si>
-    <t>def start_training():</t>
-  </si>
-  <si>
-    <t>Starts a training session for a specified dataset. Sends a command to all clients to prepare for training. Uses threading to wait until all clients are ready before starting the training.</t>
-  </si>
-  <si>
-    <t>def prepare_training():</t>
-  </si>
-  <si>
-    <t>Prepares the server-side setup for a client to train on a specified dataset. Marks the client as ready once the preparation is complete.</t>
-  </si>
-  <si>
-    <t>def wait_and_start_clients(dataset):</t>
-  </si>
-  <si>
-    <t>A helper function that waits for all clients to be ready before sending the start training signal to each client. Ensures that training only begins when all clients are synchronized.</t>
-  </si>
-  <si>
-    <t>def update_client_status():</t>
-  </si>
-  <si>
-    <t>Updates the status of a client on the server (e.g., ready, training, etc.) based on the information sent by the client.</t>
-  </si>
-  <si>
-    <t>def debug_clients():</t>
-  </si>
-  <si>
-    <t>Provides a debug endpoint that returns the current state of all registered clients in JSON format, useful for debugging and monitoring the server's state.</t>
-  </si>
-  <si>
-    <t>def set_refresh():</t>
-  </si>
-  <si>
-    <t>def clear_refresh():</t>
-  </si>
-  <si>
-    <t>def should_refresh():</t>
-  </si>
-  <si>
-    <t>def reset():</t>
-  </si>
-  <si>
-    <t>Resets the server state, including the global model, metrics, and client statuses. Notifies all clients to reset as well and triggers a server refresh.</t>
-  </si>
-  <si>
-    <t>def shutdown():</t>
-  </si>
-  <si>
-    <t>Waits until all clients are ready before initiating the training process. This function ensures synchronization across clients, preventing any client from starting too early.</t>
-  </si>
-  <si>
-    <t>def app.run(debug=True, port=5000):</t>
-  </si>
-  <si>
-    <t>def load_data(client_id, scenario):</t>
-  </si>
-  <si>
     <t>Loads and preprocesses the dataset for a given client and scenario. Supports both IID and non-IID data for technological scenarios. Returns split training and validation sets.</t>
   </si>
   <si>
-    <t>def load_medical_data_iid(client_id):</t>
-  </si>
-  <si>
-    <t>def load_medical_data_non_iid(client_id):</t>
-  </si>
-  <si>
-    <t>def create_simple_model(dataset):</t>
-  </si>
-  <si>
     <t>Creates and returns a simple model architecture based on the dataset type (technological or medical). Uses sequential layers, including dense layers for technological datasets and convolutional layers for medical datasets.</t>
   </si>
   <si>
@@ -920,554 +826,360 @@
     <t>Initiates the training process on the client upon receiving the command from the server. Starts a new training thread after verifying that the client is ready. Updates the server with the client’s status.</t>
   </si>
   <si>
-    <t>def run_training(dataset):</t>
-  </si>
-  <si>
     <t>Performs the actual model training based on the loaded dataset. After training, it sends the updated model weights and metrics back to the server. It also handles any exceptions that occur during training and ensures the training status is properly managed.</t>
   </si>
   <si>
-    <t>def compile_model(dataset):</t>
-  </si>
-  <si>
     <t>Compiles the model with an appropriate loss function and optimizer based on the dataset type. Ensures the model is ready for training.</t>
   </si>
   <si>
-    <t>def send_update(model, client_id, server_url, metrics, round_counter):</t>
-  </si>
-  <si>
     <t>Sends the updated model weights and training metrics to the server after a training round is completed.</t>
   </si>
   <si>
-    <t>def receive_model():</t>
-  </si>
-  <si>
     <t>Receives the global model weights from the server, updates the local model, and prepares the client for the next round of training. Logs the reception of the model and updates the client's status.</t>
   </si>
   <si>
-    <t>def reset_client():</t>
-  </si>
-  <si>
     <t>Resets the client’s state, including reloading the dataset, resetting the round counter, and re-registering the client with the server. Ensures the client is ready for the next round of training after a reset.</t>
   </si>
   <si>
     <t>Handles the shutdown command sent by the server, triggering the client to stop its operations.</t>
   </si>
   <si>
-    <t>def shutdown_server():</t>
-  </si>
-  <si>
     <t>Forcefully stops the Flask server running the client, ensuring that the client process is terminated immediately.</t>
   </si>
   <si>
-    <t>def app.run(debug=True, host=args.host, port=args.port):</t>
+    <t>Functions client.py</t>
+  </si>
+  <si>
+    <t>Functions server.py</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>HTTP Method</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/client_ready</t>
+  </si>
+  <si>
+    <t>/update</t>
+  </si>
+  <si>
+    <t>/start_training</t>
+  </si>
+  <si>
+    <t>/prepare_training</t>
+  </si>
+  <si>
+    <t>/client_status</t>
+  </si>
+  <si>
+    <t>/should_refresh</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/reset_server</t>
+  </si>
+  <si>
+    <t>/shutdown</t>
+  </si>
+  <si>
+    <t>/debug/clients</t>
+  </si>
+  <si>
+    <t>/receive_model</t>
+  </si>
+  <si>
+    <t>/reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML </t>
+  </si>
+  <si>
+    <t>Hypertext Markup Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESTful API </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON </t>
+  </si>
+  <si>
+    <t>Hypertext Transfer Protocol</t>
+  </si>
+  <si>
+    <t>Representational State Transfer Application Programming Interface</t>
+  </si>
+  <si>
+    <t>JavaScript Object Notation</t>
+  </si>
+  <si>
+    <t>register_client()</t>
+  </si>
+  <si>
+    <t>Registers a client with the server, storing their details (ID, port, host) in a dictionary. Triggers a refresh if all expected clients (5) are registered.</t>
+  </si>
+  <si>
+    <t>client_ready()</t>
+  </si>
+  <si>
+    <t>Updates the status of a registered client to 'ready' when the client notifies the server that it is ready.</t>
+  </si>
+  <si>
+    <t>prepare_training()</t>
+  </si>
+  <si>
+    <t>Prepares a specific client for training by setting its status to 'ready' and logging the preparation.</t>
+  </si>
+  <si>
+    <t>wait_and_start_clients()</t>
+  </si>
+  <si>
+    <t>Waits until all clients are ready and then sends a request to each client to start training with the specified dataset.</t>
+  </si>
+  <si>
+    <t>start_training()</t>
+  </si>
+  <si>
+    <t>Initiates the training process by preparing all clients and starting training once they are ready. It creates a thread to handle training when all clients are ready.</t>
+  </si>
+  <si>
+    <t>handle_medical_training_communication()</t>
+  </si>
+  <si>
+    <t>Handles communication for the medical training scenario, ensuring that all clients are ready before starting the training. Retries if communication fails, and logs the outcome.</t>
+  </si>
+  <si>
+    <t>start_medical_training()</t>
+  </si>
+  <si>
+    <t>Starts the medical training process by calling handle_medical_training_communication(). Returns success or failure based on client synchronization.</t>
+  </si>
+  <si>
+    <t>update_model()</t>
+  </si>
+  <si>
+    <t>Receives model updates from clients, stores the updates, and triggers model aggregation when all clients have submitted their updates for the current round.</t>
+  </si>
+  <si>
+    <t>aggregate_models()</t>
+  </si>
+  <si>
+    <t>Aggregates the models from all clients by averaging their weights and metrics. Updates the global model and cumulative metrics, resets client statuses, and triggers a server refresh.</t>
+  </si>
+  <si>
+    <t>update_client_status()</t>
+  </si>
+  <si>
+    <t>Updates a client's status on the server (e.g., to 'training') and triggers a server refresh if needed.</t>
+  </si>
+  <si>
+    <t>debug_clients()</t>
+  </si>
+  <si>
+    <t>Returns the current state of all registered clients for debugging purposes.</t>
+  </si>
+  <si>
+    <t>set_refresh()</t>
+  </si>
+  <si>
+    <t>Sets the refresh flag to True, indicating that the server should trigger a refresh.</t>
+  </si>
+  <si>
+    <t>clear_refresh()</t>
+  </si>
+  <si>
+    <t>Clears the refresh flag, indicating that the server has completed its refresh.</t>
+  </si>
+  <si>
+    <t>should_refresh()</t>
+  </si>
+  <si>
+    <t>Returns the current state of the refresh flag (True or False). Clears the flag after returning True.</t>
+  </si>
+  <si>
+    <t>reset()</t>
+  </si>
+  <si>
+    <t>Resets the server's state, clearing the global model, metrics, and round counters. It also sends a reset request to all clients and triggers a server refresh.</t>
+  </si>
+  <si>
+    <t>index()</t>
+  </si>
+  <si>
+    <t>Renders the main web page, showing the status of clients and the averaged metrics across all rounds.</t>
+  </si>
+  <si>
+    <t>shutdown()</t>
+  </si>
+  <si>
+    <t>Notifies all clients of the server's shutdown and then forcefully stops the server.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prepare_training()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> start_training()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> receive_model()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reset_client()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shutdown()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shutdown_server()</t>
+  </si>
+  <si>
+    <t>compile_model(dataset)</t>
+  </si>
+  <si>
+    <t>receive_model()</t>
+  </si>
+  <si>
+    <t>reset_client()</t>
+  </si>
+  <si>
+    <t>shutdown_server()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> load_medical_data_iid()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> load_data()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> load_medical_data_non_iid()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> create_simple_model()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> run_training()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> compile_model()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> send_update()</t>
+  </si>
+  <si>
+    <t>load_data()</t>
+  </si>
+  <si>
+    <t>load_medical_data_iid()</t>
+  </si>
+  <si>
+    <t>load_medical_data_non_iid()</t>
+  </si>
+  <si>
+    <t>create_simple_model()</t>
+  </si>
+  <si>
+    <t>run_training()</t>
+  </si>
+  <si>
+    <t>send_update()</t>
+  </si>
+  <si>
+    <t>Loads IID medical image data for a specified client, preparing it for training using ImageDataGenerator. Returns training and testing data generators.</t>
+  </si>
+  <si>
+    <t>Loads non-IID medical image data for a specified client, similar to load_medical_data_iid, but for non-IID scenarios. Returns training and testing data generators.</t>
+  </si>
+  <si>
+    <t>Defined in server.py</t>
+  </si>
+  <si>
+    <t>Defined in client.py</t>
+  </si>
+  <si>
+    <t>Called by server.py</t>
+  </si>
+  <si>
+    <t>Called by client.py</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Clients use this endpoint to register with the server.</t>
+  </si>
+  <si>
+    <t>Clients notify the server that they are ready to start the training process.</t>
+  </si>
+  <si>
+    <t>Server instructs clients to prepare for training; clients handle preparation.</t>
+  </si>
+  <si>
+    <t>Clients are instructed by the server to start training; clients initiate training.</t>
+  </si>
+  <si>
+    <t>Clients send their local model updates to the server for aggregation.</t>
+  </si>
+  <si>
+    <t>Clients receive the updated global model from the server.</t>
+  </si>
+  <si>
+    <t>Clients reset their state in preparation for a new training cycle.</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Sets the global </t>
+      <t xml:space="preserve">Server resets its state and instructs clients to reset through their </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <rFont val="Arial Unicode MS"/>
       </rPr>
-      <t>should_refresh</t>
+      <t>/reset</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> flag to </t>
+      <t>.</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>True</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, indicating that a page refresh is needed to reflect the latest server state.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Resets the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>should_refresh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> flag to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>False</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> after a refresh has been triggered, ensuring that the refresh state is only active when needed.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Provides an endpoint that checks if the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>should_refresh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> flag is set. If so, it returns </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>True</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and resets the flag, prompting a page refresh on the client-side.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Notifies all connected clients that the server is shutting down and then gracefully stops the server. It uses </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>os._exit(0)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> to immediately stop the server, ensuring no lingering processes.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Runs the Flask application, initializing the server on port 5000. The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>debug=True</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> option is set for development purposes, allowing for easier debugging and automatic reloading during development.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Loads IID medical image data for a specified client, preparing it for training using </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ImageDataGenerator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>. Returns training and testing data generators.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Loads non-IID medical image data for a specified client, similar to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>load_medical_data_iid</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, but for non-IID scenarios. Returns training and testing data generators.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Starts the Flask application, initializing the client on the specified host and port. The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>debug=True</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> option is set for development purposes, allowing for easier debugging and automatic reloading during development.</t>
-    </r>
-  </si>
-  <si>
-    <t>Functions client.py</t>
-  </si>
-  <si>
-    <t>Functions server.py</t>
-  </si>
-  <si>
-    <t>Endpoint</t>
-  </si>
-  <si>
-    <t>HTTP Method</t>
-  </si>
-  <si>
-    <t>server.py</t>
-  </si>
-  <si>
-    <t>client.py</t>
-  </si>
-  <si>
-    <t>/register</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>Clients register themselves with the server by sending their ID, port, and host details.</t>
-  </si>
-  <si>
-    <t>Registers the client and updates server state.</t>
-  </si>
-  <si>
-    <t>Sends client details to the server for registration.</t>
-  </si>
-  <si>
-    <t>/client_ready</t>
-  </si>
-  <si>
-    <t>Clients notify the server that they are ready to begin training.</t>
-  </si>
-  <si>
-    <t>Updates client status to 'ready'.</t>
-  </si>
-  <si>
-    <t>Sends readiness status to the server.</t>
-  </si>
-  <si>
-    <t>/update</t>
-  </si>
-  <si>
-    <t>Clients send their model updates (weights and metrics) to the server after a training round.</t>
-  </si>
-  <si>
-    <t>Receives model updates and aggregates them.</t>
-  </si>
-  <si>
-    <t>Sends updated model weights and metrics to the server.</t>
-  </si>
-  <si>
-    <t>/start_training</t>
-  </si>
-  <si>
-    <t>The server sends a command to all clients to start the training process for a specific dataset.</t>
-  </si>
-  <si>
-    <t>Initiates training for all clients.</t>
-  </si>
-  <si>
-    <t>Receives start command and begins local training.</t>
-  </si>
-  <si>
-    <t>/prepare_training</t>
-  </si>
-  <si>
-    <t>The server instructs a specific client to prepare for training with a designated dataset.</t>
-  </si>
-  <si>
-    <t>Sends preparation command to specific client.</t>
-  </si>
-  <si>
-    <t>Prepares client for training based on the received dataset.</t>
-  </si>
-  <si>
-    <t>/client_status</t>
-  </si>
-  <si>
-    <t>Updates the status of a client on the server (e.g., ready, training).</t>
-  </si>
-  <si>
-    <t>Updates the status of a specific client.</t>
-  </si>
-  <si>
-    <t>Sends the current client status to the server.</t>
-  </si>
-  <si>
-    <t>/should_refresh</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>Clients check whether they need to refresh their state based on server-side changes.</t>
-  </si>
-  <si>
-    <t>Indicates whether a refresh is required.</t>
-  </si>
-  <si>
-    <t>/reset_server</t>
-  </si>
-  <si>
-    <t>Resets the server's state, including the global model, metrics, and client statuses.</t>
-  </si>
-  <si>
-    <t>Resets server and notifies clients.</t>
-  </si>
-  <si>
-    <t>/shutdown</t>
-  </si>
-  <si>
-    <t>The server sends a shutdown command to all connected clients, then stops itself.</t>
-  </si>
-  <si>
-    <t>Shuts down the server and notifies clients.</t>
-  </si>
-  <si>
-    <t>Receives shutdown command and stops client operations.</t>
-  </si>
-  <si>
-    <t>/debug/clients</t>
-  </si>
-  <si>
-    <t>Provides a debug endpoint that returns the current state of all registered clients.</t>
-  </si>
-  <si>
-    <t>Returns the current state of all clients.</t>
-  </si>
-  <si>
-    <t>/receive_model</t>
-  </si>
-  <si>
-    <t>Receives the global model weights from the server and updates the local model.</t>
-  </si>
-  <si>
-    <t>Sends updated global model weights to clients.</t>
-  </si>
-  <si>
-    <t>Receives updated global model weights from the server.</t>
-  </si>
-  <si>
-    <t>/reset</t>
-  </si>
-  <si>
-    <t>Resets the client’s state and prepares it for the next round of training.</t>
-  </si>
-  <si>
-    <t>Sends reset command to clients.</t>
-  </si>
-  <si>
-    <t>Resets the client state and re-registers with the server</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTML </t>
-  </si>
-  <si>
-    <t>Hypertext Markup Language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTTP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESTful API </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JSON </t>
-  </si>
-  <si>
-    <t>Hypertext Transfer Protocol</t>
-  </si>
-  <si>
-    <t>Representational State Transfer Application Programming Interface</t>
-  </si>
-  <si>
-    <t>JavaScript Object Notation</t>
-  </si>
-  <si>
-    <t>register_client():</t>
-  </si>
-  <si>
-    <t>client_ready():</t>
-  </si>
-  <si>
-    <t>prepare_training():</t>
-  </si>
-  <si>
-    <t>update_model():</t>
-  </si>
-  <si>
-    <t>aggregate_models(client_updates):</t>
-  </si>
-  <si>
-    <t>index():</t>
-  </si>
-  <si>
-    <t>start_training():</t>
-  </si>
-  <si>
-    <t>wait_and_start_clients(dataset):</t>
-  </si>
-  <si>
-    <t>set_refresh():</t>
-  </si>
-  <si>
-    <t>clear_refresh():</t>
-  </si>
-  <si>
-    <t>should_refresh():</t>
-  </si>
-  <si>
-    <t>reset():</t>
-  </si>
-  <si>
-    <t>shutdown():</t>
-  </si>
-  <si>
-    <t>debug_clients():</t>
-  </si>
-  <si>
-    <t>update_client_status():</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> load_data(client_id, scenario):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> load_medical_data_iid(client_id):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> load_medical_data_non_iid(client_id):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> create_simple_model(dataset):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> prepare_training():</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> start_training():</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> run_training(dataset):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> compile_model(dataset):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> send_update(model, client_id, server_url, metrics, round_counter):</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> receive_model():</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> reset_client():</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> shutdown():</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> shutdown_server():</t>
+  </si>
+  <si>
+    <t>Both server and clients can initiate shutdown sequences.</t>
+  </si>
+  <si>
+    <t>Clients can check if they need to refresh their state or restart training.</t>
+  </si>
+  <si>
+    <t>Clients update the server with their current status (e.g., "training").</t>
+  </si>
+  <si>
+    <t>/start_medical_training</t>
+  </si>
+  <si>
+    <t>Server specifically handles the start of the medical training process.</t>
+  </si>
+  <si>
+    <t>Used for debugging; this endpoint returns the current state of all clients</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1517,6 +1229,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1617,7 +1334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1694,10 +1411,10 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1736,14 +1453,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2088,13 +1797,13 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2102,7 +1811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>103</v>
       </c>
@@ -2110,7 +1819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>152</v>
       </c>
@@ -2118,7 +1827,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>187</v>
       </c>
@@ -2126,7 +1835,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>89</v>
       </c>
@@ -2134,7 +1843,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>150</v>
       </c>
@@ -2142,7 +1851,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2150,7 +1859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -2158,7 +1867,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -2166,7 +1875,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2174,7 +1883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>189</v>
       </c>
@@ -2182,7 +1891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -2190,7 +1899,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -2198,7 +1907,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2214,7 +1923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>93</v>
       </c>
@@ -2222,7 +1931,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2230,23 +1939,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>327</v>
+        <v>244</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>329</v>
+        <v>246</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2254,7 +1963,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>185</v>
       </c>
@@ -2262,15 +1971,15 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
@@ -2278,7 +1987,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2286,7 +1995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -2294,7 +2003,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -2302,7 +2011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>146</v>
       </c>
@@ -2310,7 +2019,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>154</v>
       </c>
@@ -2318,15 +2027,15 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>330</v>
+        <v>247</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>156</v>
       </c>
@@ -2334,7 +2043,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>148</v>
       </c>
@@ -2342,7 +2051,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
@@ -2350,7 +2059,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2358,7 +2067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -2387,12 +2096,12 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="6" width="52.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:6">
       <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
         <v>172</v>
@@ -2401,7 +2110,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:6" ht="28.8">
       <c r="D5" s="21"/>
       <c r="E5" s="4" t="s">
         <v>174</v>
@@ -2410,7 +2119,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:6" ht="28.8">
       <c r="D6" s="21"/>
       <c r="E6" s="4" t="s">
         <v>175</v>
@@ -2419,7 +2128,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:6" ht="28.8">
       <c r="D7" s="21"/>
       <c r="E7" s="4" t="s">
         <v>176</v>
@@ -2428,7 +2137,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:6" ht="28.8">
       <c r="D8" s="21"/>
       <c r="E8" s="4" t="s">
         <v>177</v>
@@ -2437,7 +2146,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:6" ht="28.8">
       <c r="D9" s="21"/>
       <c r="E9" s="4" t="s">
         <v>178</v>
@@ -2446,7 +2155,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:6" ht="28.8">
       <c r="D10" s="21"/>
       <c r="E10" s="4">
         <v>10</v>
@@ -2468,7 +2177,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.109375" customWidth="1"/>
@@ -2478,7 +2187,7 @@
     <col min="15" max="15" width="130.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:15" ht="28.8">
       <c r="D4" s="40"/>
       <c r="E4" s="40"/>
       <c r="F4" s="41"/>
@@ -2497,7 +2206,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="4:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:15" ht="43.2">
       <c r="D5" s="4" t="s">
         <v>190</v>
       </c>
@@ -2526,7 +2235,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:15">
       <c r="D6" s="12" t="s">
         <v>198</v>
       </c>
@@ -2555,7 +2264,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:15">
       <c r="D7" s="12" t="s">
         <v>199</v>
       </c>
@@ -2584,7 +2293,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="8" spans="4:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:15" ht="28.8">
       <c r="D8" s="12" t="s">
         <v>200</v>
       </c>
@@ -2613,7 +2322,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:15">
       <c r="D9" s="12" t="s">
         <v>201</v>
       </c>
@@ -2642,7 +2351,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:15">
       <c r="D10" s="12" t="s">
         <v>202</v>
       </c>
@@ -2671,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:15">
       <c r="E14" s="15"/>
       <c r="F14" s="25"/>
       <c r="G14" s="26"/>
@@ -2681,7 +2390,7 @@
       <c r="K14" s="26"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:6">
       <c r="E17" s="15"/>
       <c r="F17" s="26"/>
     </row>
@@ -2703,7 +2412,7 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.109375" customWidth="1"/>
@@ -2713,7 +2422,7 @@
     <col min="14" max="14" width="130.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:14" ht="28.8">
       <c r="D4" s="40"/>
       <c r="E4" s="40"/>
       <c r="F4" s="41"/>
@@ -2730,7 +2439,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:14" ht="28.8">
       <c r="D5" s="4" t="s">
         <v>190</v>
       </c>
@@ -2754,7 +2463,7 @@
       </c>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:14">
       <c r="D6" s="12" t="s">
         <v>198</v>
       </c>
@@ -2779,7 +2488,7 @@
       </c>
       <c r="K6" s="26"/>
     </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:14">
       <c r="D7" s="12" t="s">
         <v>199</v>
       </c>
@@ -2804,7 +2513,7 @@
       </c>
       <c r="K7" s="26"/>
     </row>
-    <row r="8" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:14" ht="28.8">
       <c r="D8" s="12" t="s">
         <v>200</v>
       </c>
@@ -2829,7 +2538,7 @@
       </c>
       <c r="K8" s="26"/>
     </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:14">
       <c r="D9" s="12" t="s">
         <v>201</v>
       </c>
@@ -2854,7 +2563,7 @@
       </c>
       <c r="K9" s="26"/>
     </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:14">
       <c r="D10" s="12" t="s">
         <v>202</v>
       </c>
@@ -2879,7 +2588,7 @@
       </c>
       <c r="K10" s="26"/>
     </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:14">
       <c r="E14" s="15"/>
       <c r="F14" s="25"/>
       <c r="G14" s="26"/>
@@ -2888,7 +2597,7 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:6">
       <c r="E17" s="15"/>
       <c r="F17" s="26"/>
     </row>
@@ -2903,111 +2612,121 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D28749-D765-415A-9C12-E1FE75AF4B71}">
-  <dimension ref="C3:F18"/>
+  <dimension ref="B3:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="45" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" style="42" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="43"/>
-      <c r="F3" s="4" t="s">
+    <row r="3" spans="2:3">
+      <c r="B3" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="29"/>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="29"/>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="29"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="29"/>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="C12" s="29"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" s="29"/>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14" s="29"/>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="28" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="44"/>
-      <c r="F4" s="29" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="44"/>
-      <c r="F5" s="29" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="44"/>
-      <c r="F6" s="29" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="44"/>
-      <c r="F7" s="29" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="44"/>
-      <c r="F8" s="29" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="44"/>
-      <c r="F9" s="29" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="44"/>
-      <c r="F10" s="29" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="44"/>
-      <c r="F11" s="29" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="44"/>
-      <c r="F12" s="29" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="44"/>
-      <c r="F13" s="29" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="44"/>
-      <c r="F14" s="29" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="F15" s="29" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="F16" s="29" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="44"/>
-      <c r="F17" s="29" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="44"/>
-      <c r="F18" s="29" t="s">
-        <v>347</v>
+    <row r="16" spans="2:3">
+      <c r="B16" s="28" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="C17" s="29"/>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="28" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="28" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3017,160 +2736,160 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE30FFEC-DD3A-43C2-9692-82381583DFB4}">
-  <dimension ref="C3:D20"/>
+  <dimension ref="D3:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="4:5">
+      <c r="D3" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="43.2">
+      <c r="D4" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="28.8">
+      <c r="D5" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="28.8">
+      <c r="D6" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" ht="43.2">
+      <c r="D7" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="57.6">
+      <c r="D8" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="57.6">
+      <c r="D9" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" ht="57.6">
+      <c r="D10" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" ht="57.6">
+      <c r="D11" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" ht="57.6">
+      <c r="D12" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="28.8">
+      <c r="D13" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" ht="28.8">
+      <c r="D14" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" ht="28.8">
+      <c r="D15" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C4" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C6" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C9" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C10" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C11" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C12" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C13" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C14" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C15" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C16" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C17" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C18" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C19" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>269</v>
+      <c r="E15" s="28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" ht="28.8">
+      <c r="D16" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="28.8">
+      <c r="D17" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" ht="57.6">
+      <c r="D18" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" ht="43.2">
+      <c r="D19" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" ht="28.8">
+      <c r="D20" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3179,137 +2898,87 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1877F309-2AC0-4525-B1B7-2FED63E9E5D6}">
-  <dimension ref="C3:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D455F8B2-ECEE-4F97-AE0E-F30B6212FF7D}">
+  <dimension ref="C3:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:3">
       <c r="C3" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3">
       <c r="C4" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
       <c r="C5" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3">
       <c r="C6" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" ht="72" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3">
       <c r="C7" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
       <c r="C8" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3">
       <c r="C9" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" ht="72" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3">
       <c r="C10" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3">
       <c r="C11" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3">
       <c r="C12" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
       <c r="C13" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
       <c r="C14" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3">
       <c r="C15" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
       <c r="C16" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="C17" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3318,87 +2987,129 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D455F8B2-ECEE-4F97-AE0E-F30B6212FF7D}">
-  <dimension ref="C3:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1877F309-2AC0-4525-B1B7-2FED63E9E5D6}">
+  <dimension ref="C3:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="55.21875" customWidth="1"/>
-    <col min="5" max="5" width="55.5546875" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:4">
       <c r="C3" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="29" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="29" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C6" s="29" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="29" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C8" s="29" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="29" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C10" s="29" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C11" s="29" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C12" s="29" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C13" s="29" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C14" s="29" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C15" s="29" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C16" s="29" t="s">
-        <v>362</v>
+        <v>226</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="57.6">
+      <c r="C4" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="43.2">
+      <c r="C5" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="57.6">
+      <c r="C6" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="72">
+      <c r="C7" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="57.6">
+      <c r="C8" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="57.6">
+      <c r="C9" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="72">
+      <c r="C10" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="43.2">
+      <c r="C11" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="28.8">
+      <c r="C12" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="57.6">
+      <c r="C13" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="57.6">
+      <c r="C14" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="28.8">
+      <c r="C15" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="43.2">
+      <c r="C16" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3407,244 +3118,652 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A9E57B-1589-46D6-912B-B22AAF95984C}">
+  <dimension ref="F4:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:11" ht="28.8">
+      <c r="F4" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="6:11">
+      <c r="F5" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="6:11">
+      <c r="F6" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="6:11">
+      <c r="F7" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="6:11">
+      <c r="F8" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="6:11">
+      <c r="F9" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="6:11">
+      <c r="F10" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="6:11">
+      <c r="F11" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="6:11">
+      <c r="F12" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="13" spans="6:11">
+      <c r="F13" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="6:11">
+      <c r="F14" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="6:11">
+      <c r="F15" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="16" spans="6:11">
+      <c r="F16" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11">
+      <c r="F17" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
-  <dimension ref="C3:G15"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="E3:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E4" sqref="E4:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>276</v>
-      </c>
+    <row r="3" spans="5:11" ht="28.8">
       <c r="E3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C4" s="28" t="s">
-        <v>279</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>281</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="28" t="s">
-        <v>288</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>289</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C7" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C8" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>297</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C9" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>306</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="G10" s="29" t="s">
+    </row>
+    <row r="4" spans="5:11" ht="28.8">
+      <c r="E4" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="5:11" ht="43.2">
+      <c r="E5" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="5:11" ht="43.2">
+      <c r="E6" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="5:11" ht="43.2">
+      <c r="E7" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="5:11" ht="43.2">
+      <c r="E8" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" ht="43.2">
+      <c r="E9" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" ht="43.2" hidden="1">
+      <c r="E10" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" ht="43.2" hidden="1">
+      <c r="E11" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11" ht="43.2">
+      <c r="E12" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="5:11" ht="28.8">
+      <c r="E13" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11" ht="43.2">
+      <c r="E14" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K14" s="28" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="28" t="s">
-        <v>308</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>310</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C12" s="28" t="s">
-        <v>311</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>313</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="E13" s="29" t="s">
+    <row r="15" spans="5:11" ht="43.2">
+      <c r="E15" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="F13" s="29" t="s">
-        <v>317</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C14" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>319</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>325</v>
+      <c r="I15" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="5:11" ht="43.2">
+      <c r="E16" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E3:K16" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3657,14 +3776,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
     <col min="6" max="6" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:6">
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
         <v>1</v>
@@ -3673,7 +3792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:6" ht="57.6">
       <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
@@ -3684,7 +3803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:6" ht="72">
       <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
@@ -3695,7 +3814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:6" ht="86.4">
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
@@ -3706,7 +3825,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:6" ht="72">
       <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
@@ -3731,7 +3850,7 @@
       <selection activeCell="O4" sqref="O4:W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
@@ -3751,7 +3870,7 @@
     <col min="23" max="23" width="48.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:23" ht="28.8">
       <c r="C4" s="4" t="s">
         <v>37</v>
       </c>
@@ -3807,7 +3926,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:23">
       <c r="C5" s="4" t="s">
         <v>45</v>
       </c>
@@ -3867,7 +3986,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:23">
       <c r="C6" s="4" t="s">
         <v>44</v>
       </c>
@@ -3927,7 +4046,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:23">
       <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
@@ -3987,7 +4106,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:23">
       <c r="C8" s="4" t="s">
         <v>58</v>
       </c>
@@ -4047,7 +4166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:23">
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
@@ -4107,7 +4226,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:23">
       <c r="C10" s="4" t="s">
         <v>46</v>
       </c>
@@ -4167,7 +4286,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:23">
       <c r="C11" s="4" t="s">
         <v>41</v>
       </c>
@@ -4227,7 +4346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:23">
       <c r="C12" s="4" t="s">
         <v>56</v>
       </c>
@@ -4287,7 +4406,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:23">
       <c r="C13" s="4" t="s">
         <v>43</v>
       </c>
@@ -4347,7 +4466,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="3:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:23">
       <c r="C14" s="4" t="s">
         <v>47</v>
       </c>
@@ -4407,7 +4526,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="3:23" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:23" ht="19.2" customHeight="1">
       <c r="C15" s="30" t="s">
         <v>67</v>
       </c>
@@ -4431,7 +4550,7 @@
       <c r="V15" s="33"/>
       <c r="W15" s="33"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6">
       <c r="C18" t="s">
         <v>60</v>
       </c>
@@ -4448,7 +4567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6">
       <c r="C19" t="s">
         <v>61</v>
       </c>
@@ -4485,14 +4604,14 @@
       <selection activeCell="D14" sqref="D14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="41.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:6">
       <c r="D3" s="4" t="s">
         <v>79</v>
       </c>
@@ -4503,7 +4622,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:6">
       <c r="D4" s="13" t="s">
         <v>82</v>
       </c>
@@ -4514,7 +4633,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:6">
       <c r="D5" s="13" t="s">
         <v>82</v>
       </c>
@@ -4525,7 +4644,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:6">
       <c r="D6" s="13" t="s">
         <v>82</v>
       </c>
@@ -4536,7 +4655,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:6">
       <c r="D7" s="13" t="s">
         <v>82</v>
       </c>
@@ -4547,7 +4666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:6">
       <c r="D8" s="13" t="s">
         <v>80</v>
       </c>
@@ -4558,7 +4677,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:6" ht="28.8">
       <c r="D9" s="13" t="s">
         <v>85</v>
       </c>
@@ -4569,7 +4688,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:6">
       <c r="D10" s="13" t="s">
         <v>85</v>
       </c>
@@ -4580,7 +4699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:6">
       <c r="D11" s="13" t="s">
         <v>81</v>
       </c>
@@ -4591,7 +4710,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:6">
       <c r="D12" s="13" t="s">
         <v>84</v>
       </c>
@@ -4602,7 +4721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:6" ht="28.8">
       <c r="D13" s="13" t="s">
         <v>83</v>
       </c>
@@ -4613,7 +4732,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="4:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:6" ht="14.4" customHeight="1">
       <c r="D14" s="34" t="s">
         <v>67</v>
       </c>
@@ -4639,13 +4758,13 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="5" width="23.109375" customWidth="1"/>
     <col min="6" max="6" width="46.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:6">
       <c r="E5" s="4" t="s">
         <v>95</v>
       </c>
@@ -4653,7 +4772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="5:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:6" ht="57.6">
       <c r="E6" s="4" t="s">
         <v>82</v>
       </c>
@@ -4661,7 +4780,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="5:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:6" ht="43.2">
       <c r="E7" s="4" t="s">
         <v>96</v>
       </c>
@@ -4669,7 +4788,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="5:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:6" ht="43.2">
       <c r="E8" s="4" t="s">
         <v>87</v>
       </c>
@@ -4677,7 +4796,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="5:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:6" ht="43.2">
       <c r="E9" s="4" t="s">
         <v>98</v>
       </c>
@@ -4685,7 +4804,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:6">
       <c r="F14" s="14"/>
     </row>
   </sheetData>
@@ -4701,7 +4820,7 @@
       <selection activeCell="I3" sqref="I3:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" hidden="1" customWidth="1"/>
@@ -4710,11 +4829,11 @@
     <col min="9" max="9" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="G2" s="4" t="s">
@@ -4727,7 +4846,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="G3" s="17" t="s">
@@ -4740,7 +4859,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="28.8">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="G4" s="17" t="s">
@@ -4753,7 +4872,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="G5" s="17" t="s">
@@ -4766,7 +4885,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="G6" s="17" t="s">
@@ -4779,7 +4898,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="G7" s="17" t="s">
@@ -4792,7 +4911,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="G8" s="17" t="s">
@@ -4805,7 +4924,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="G9" s="17" t="s">
@@ -4818,7 +4937,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="G10" s="17" t="s">
@@ -4831,7 +4950,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="G11" s="17" t="s">
@@ -4844,7 +4963,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="G12" s="17" t="s">
         <v>115</v>
       </c>
@@ -4855,7 +4974,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="G13" s="34" t="s">
         <v>67</v>
       </c>
@@ -4881,13 +5000,13 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="123.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="6:7">
       <c r="F3" s="4" t="s">
         <v>116</v>
       </c>
@@ -4895,7 +5014,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="6:7" ht="15" customHeight="1">
       <c r="F4" s="4" t="s">
         <v>118</v>
       </c>
@@ -4903,7 +5022,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="6:7" ht="15" customHeight="1">
       <c r="F5" s="4" t="s">
         <v>119</v>
       </c>
@@ -4911,7 +5030,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:7" ht="15" customHeight="1">
       <c r="F6" s="4" t="s">
         <v>121</v>
       </c>
@@ -4919,7 +5038,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="6:7" ht="15" customHeight="1">
       <c r="F7" s="4" t="s">
         <v>123</v>
       </c>
@@ -4927,7 +5046,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="6:7" ht="15" customHeight="1">
       <c r="F8" s="4" t="s">
         <v>125</v>
       </c>
@@ -4935,7 +5054,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:7" ht="15" customHeight="1">
       <c r="F9" s="4" t="s">
         <v>127</v>
       </c>
@@ -4943,7 +5062,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:7" ht="15" customHeight="1">
       <c r="F10" s="4" t="s">
         <v>129</v>
       </c>
@@ -4951,7 +5070,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="6:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="6:7" ht="57.6">
       <c r="F11" s="4" t="s">
         <v>130</v>
       </c>
@@ -4959,7 +5078,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:7" ht="28.8">
       <c r="F12" s="4" t="s">
         <v>131</v>
       </c>
@@ -4967,7 +5086,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:7">
       <c r="F13" s="4" t="s">
         <v>133</v>
       </c>
@@ -4975,7 +5094,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="6:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:7" ht="43.2">
       <c r="F14" s="4" t="s">
         <v>135</v>
       </c>
@@ -4983,7 +5102,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:7" ht="28.8">
       <c r="F15" s="4" t="s">
         <v>137</v>
       </c>
@@ -4991,7 +5110,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="6:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:7" ht="28.8">
       <c r="F16" s="4" t="s">
         <v>139</v>
       </c>
@@ -4999,7 +5118,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:7">
       <c r="F17" s="4" t="s">
         <v>141</v>
       </c>
@@ -5020,14 +5139,14 @@
       <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="5" width="24.88671875" customWidth="1"/>
     <col min="6" max="6" width="53.77734375" customWidth="1"/>
     <col min="7" max="7" width="37.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:7">
       <c r="E4" s="4" t="s">
         <v>158</v>
       </c>
@@ -5036,7 +5155,7 @@
       </c>
       <c r="G4" s="33"/>
     </row>
-    <row r="5" spans="5:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:7" ht="28.8" customHeight="1">
       <c r="E5" s="4" t="s">
         <v>159</v>
       </c>
@@ -5047,14 +5166,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:7">
       <c r="E6" s="4" t="s">
         <v>160</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:7">
       <c r="E7" s="4" t="s">
         <v>161</v>
       </c>
@@ -5063,14 +5182,14 @@
       </c>
       <c r="G7" s="38"/>
     </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:7">
       <c r="E8" s="4" t="s">
         <v>162</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:7" ht="28.8">
       <c r="E9" s="4" t="s">
         <v>163</v>
       </c>
@@ -5096,7 +5215,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="5" width="6.44140625" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" hidden="1" customWidth="1"/>
@@ -5106,7 +5225,7 @@
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="7:10">
       <c r="G6" s="4" t="s">
         <v>158</v>
       </c>
@@ -5118,7 +5237,7 @@
       </c>
       <c r="J6" s="33"/>
     </row>
-    <row r="7" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="7:10">
       <c r="G7" s="4" t="s">
         <v>159</v>
       </c>
@@ -5132,7 +5251,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="7:10">
       <c r="G8" s="4" t="s">
         <v>160</v>
       </c>
@@ -5140,7 +5259,7 @@
       <c r="I8" s="37"/>
       <c r="J8" s="39"/>
     </row>
-    <row r="9" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="7:10">
       <c r="G9" s="4" t="s">
         <v>161</v>
       </c>
@@ -5150,7 +5269,7 @@
       </c>
       <c r="J9" s="39"/>
     </row>
-    <row r="10" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="7:10" ht="28.8">
       <c r="G10" s="4" t="s">
         <v>162</v>
       </c>
@@ -5160,7 +5279,7 @@
       <c r="I10" s="37"/>
       <c r="J10" s="39"/>
     </row>
-    <row r="11" spans="7:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="7:10" ht="28.8">
       <c r="G11" s="4" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Starting section 7.Results. Words left 4,068.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="973" documentId="8_{1CD4F42F-7BFE-4E5F-B8BE-5A13F6FC91AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA11D1B-AD06-4CB3-A576-9B93B7555E69}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41995BD5-2015-465A-8E60-AAD3504CA92E}"/>
   <bookViews>
-    <workbookView xWindow="48990" yWindow="150" windowWidth="17280" windowHeight="22770" tabRatio="715" firstSheet="12" activeTab="16" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView minimized="1" xWindow="1776" yWindow="156" windowWidth="17280" windowHeight="12204" tabRatio="715" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -30,11 +30,13 @@
     <sheet name="Table 6.2.2" sheetId="17" r:id="rId15"/>
     <sheet name="T.Client.py" sheetId="15" r:id="rId16"/>
     <sheet name="Table 6.3. Endpoints and HTTP" sheetId="20" r:id="rId17"/>
-    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId18"/>
+    <sheet name="Table 6.4.1. Medical model laye" sheetId="21" r:id="rId18"/>
+    <sheet name="Table 6.4.2. Technologica model" sheetId="22" r:id="rId19"/>
+    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$K$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
   </definedNames>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="358">
   <si>
     <t>FL</t>
   </si>
@@ -1180,6 +1182,87 @@
   </si>
   <si>
     <t>Used for debugging; this endpoint returns the current state of all clients</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Input Layer</t>
+  </si>
+  <si>
+    <t>Accepts images with dimensions 128x128x3 (height, width, and color channels).</t>
+  </si>
+  <si>
+    <t>First Convolutional Layer</t>
+  </si>
+  <si>
+    <t>Uses 16 filters with a 3x3 kernel size, followed by ReLU activation and padding.</t>
+  </si>
+  <si>
+    <t>Second Convolutional Layer</t>
+  </si>
+  <si>
+    <t>Uses 32 filters with a 3x3 kernel size, again with ReLU activation and padding.</t>
+  </si>
+  <si>
+    <t>Max Pooling Layers</t>
+  </si>
+  <si>
+    <t>Each convolutional layer is followed by a max pooling layer with a 2x2 pool size, reducing spatial dimensions while retaining important features.</t>
+  </si>
+  <si>
+    <t>Flatten Layer</t>
+  </si>
+  <si>
+    <t>Flattens the output of the last pooling layer to a one-dimensional vector, preparing it for the fully connected layer.</t>
+  </si>
+  <si>
+    <t>Contains 64 neurons with a ReLU activation function.</t>
+  </si>
+  <si>
+    <t>Output Layer</t>
+  </si>
+  <si>
+    <t>Comprises 2 neurons with a softmax activation function, classifying the images as "lung" or "not lung."</t>
+  </si>
+  <si>
+    <t>Fully Connected Dense Layer</t>
+  </si>
+  <si>
+    <t>Output Dense Layer</t>
+  </si>
+  <si>
+    <t>This layer comprised neurons corresponding to the seven features in the dataset.</t>
+  </si>
+  <si>
+    <t>First Hidden Layer</t>
+  </si>
+  <si>
+    <t>This layer contained 12 neurons with a ReLU activation function, and L2 regularization was applied to prevent overfitting.</t>
+  </si>
+  <si>
+    <t>Second Hidden Layer</t>
+  </si>
+  <si>
+    <t>This layer consisted of 8 neurons, also using ReLU activation and L2 regularization.</t>
+  </si>
+  <si>
+    <t>A single neuron with a sigmoid activation function was used, suitable for binary classification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federated Weighted Average </t>
+  </si>
+  <si>
+    <t>FedWAvg</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>Red, Green and Blue</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1909,175 +1992,191 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>244</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>245</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>246</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>185</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>248</v>
+        <v>185</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>251</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>92</v>
+        <v>248</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>247</v>
+        <v>154</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>157</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>148</v>
+        <v>356</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>149</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>156</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B28" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B34">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B36">
       <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
@@ -2991,7 +3090,7 @@
   <dimension ref="C3:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3121,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A9E57B-1589-46D6-912B-B22AAF95984C}">
   <dimension ref="F4:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3418,352 +3517,148 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="E3:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A837C353-FFBB-4CDE-9AA4-833F83C063F8}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E16"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:11" ht="28.8">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="D3" s="4" t="s">
+        <v>332</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>228</v>
-      </c>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8">
+      <c r="D4" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8">
+      <c r="D5" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="D6" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2">
+      <c r="D7" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2">
+      <c r="D8" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8">
+      <c r="D9" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8">
+      <c r="D10" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7298F1-C971-4635-B43B-E10502027043}">
+  <dimension ref="F3:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="40.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:7">
       <c r="F3" s="4" t="s">
-        <v>229</v>
+        <v>332</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="K3" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="5:11" ht="28.8">
-      <c r="E4" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="5:11" ht="43.2">
-      <c r="E5" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" spans="5:11" ht="43.2">
-      <c r="E6" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="7" spans="5:11" ht="43.2">
-      <c r="E7" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="5:11" ht="43.2">
-      <c r="E8" s="28" t="s">
-        <v>328</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" ht="43.2">
-      <c r="E9" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" ht="43.2" hidden="1">
-      <c r="E10" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="K10" s="28" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" ht="43.2" hidden="1">
-      <c r="E11" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="12" spans="5:11" ht="43.2">
-      <c r="E12" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="5:11" ht="28.8">
-      <c r="E13" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K13" s="28" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="14" spans="5:11" ht="43.2">
-      <c r="E14" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K14" s="28" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="15" spans="5:11" ht="43.2">
-      <c r="E15" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K15" s="28" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="16" spans="5:11" ht="43.2">
-      <c r="E16" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>330</v>
+    <row r="4" spans="6:7" ht="28.8">
+      <c r="F4" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="6:7" ht="43.2">
+      <c r="F5" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" ht="28.8">
+      <c r="F6" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="6:7" ht="43.2">
+      <c r="F7" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E3:K16" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3839,6 +3734,357 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="E3:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:11" ht="28.8">
+      <c r="E3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="5:11" ht="28.8">
+      <c r="E4" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="5:11" ht="43.2">
+      <c r="E5" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="5:11" ht="43.2">
+      <c r="E6" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="5:11" ht="43.2">
+      <c r="E7" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="5:11" ht="43.2">
+      <c r="E8" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" ht="43.2">
+      <c r="E9" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" ht="43.2" hidden="1">
+      <c r="E10" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" ht="43.2" hidden="1">
+      <c r="E11" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11" ht="43.2">
+      <c r="E12" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="5:11" ht="28.8">
+      <c r="E13" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11" ht="43.2">
+      <c r="E14" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" ht="43.2">
+      <c r="E15" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="5:11" ht="43.2">
+      <c r="E16" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>330</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="E3:K16" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4677,7 +4923,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="28.8">
+    <row r="9" spans="4:6">
       <c r="D9" s="13" t="s">
         <v>85</v>
       </c>
@@ -4721,7 +4967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.8">
+    <row r="13" spans="4:6">
       <c r="D13" s="13" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Working on section 7.1.Results.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41995BD5-2015-465A-8E60-AAD3504CA92E}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF09385E-CB44-4C15-BB7E-60809652BD36}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1776" yWindow="156" windowWidth="17280" windowHeight="12204" tabRatio="715" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="715" firstSheet="7" activeTab="20" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="Table 6.4.1. Medical model laye" sheetId="21" r:id="rId18"/>
     <sheet name="Table 6.4.2. Technologica model" sheetId="22" r:id="rId19"/>
     <sheet name="CommunicationProtocols" sheetId="18" r:id="rId20"/>
+    <sheet name="Table 7.3." sheetId="24" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="373">
   <si>
     <t>FL</t>
   </si>
@@ -1263,6 +1264,51 @@
   </si>
   <si>
     <t>Red, Green and Blue</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>H0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Null Hypothesis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shapiro Tests </t>
+  </si>
+  <si>
+    <t>ST(s)</t>
+  </si>
+  <si>
+    <t>Clients with Improved Performance</t>
+  </si>
+  <si>
+    <t>Clients with Decreased Performance</t>
+  </si>
+  <si>
+    <t>Clients with No Significant Change</t>
+  </si>
+  <si>
+    <t>Global Model Shows Improvement</t>
+  </si>
+  <si>
+    <t>Global Model Shows Decline</t>
+  </si>
+  <si>
+    <t>Technological IID</t>
+  </si>
+  <si>
+    <t>Technological Non-IID</t>
+  </si>
+  <si>
+    <t>Medical IID</t>
+  </si>
+  <si>
+    <t>Medical Non-IID</t>
   </si>
 </sst>
 </file>
@@ -1874,10 +1920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2172,6 +2218,30 @@
       </c>
       <c r="B36" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3583,7 +3653,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
+    <row r="9" spans="1:5">
       <c r="D9" s="28" t="s">
         <v>346</v>
       </c>
@@ -3743,7 +3813,7 @@
   <dimension ref="E3:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4084,6 +4154,127 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4752E1C2-D677-4722-9FF8-46C596A40F59}">
+  <dimension ref="H6:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U50" sqref="U50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="8:13" ht="43.2">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="8:13">
+      <c r="H7" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="I7" s="12">
+        <v>2</v>
+      </c>
+      <c r="J7" s="12">
+        <v>3</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="8:13">
+      <c r="H8" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="I8" s="12">
+        <v>3</v>
+      </c>
+      <c r="J8" s="12">
+        <v>2</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="8:13">
+      <c r="H9" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>5</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="8:13">
+      <c r="H10" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="I10" s="12">
+        <v>2</v>
+      </c>
+      <c r="J10" s="12">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Starting Section 4. Research and Ethics. Version 2.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4983FE81-4AD9-4466-886E-BF0FA91A44D9}"/>
+  <xr:revisionPtr revIDLastSave="273" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D8BBEA9-08C2-49C7-A61E-CB22AF2AF2CF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="715" firstSheet="6" activeTab="9" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="715" firstSheet="6" activeTab="9" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,23 @@
     <sheet name="T.3.4.1." sheetId="7" r:id="rId7"/>
     <sheet name="T.3.6." sheetId="8" r:id="rId8"/>
     <sheet name="T.3.6.1." sheetId="10" r:id="rId9"/>
-    <sheet name="T.5" sheetId="11" r:id="rId10"/>
-    <sheet name="T.5.6" sheetId="12" r:id="rId11"/>
-    <sheet name="T.6 (2)" sheetId="13" r:id="rId12"/>
-    <sheet name="Table 6.3.1" sheetId="16" r:id="rId13"/>
-    <sheet name="T.Server.py" sheetId="14" r:id="rId14"/>
-    <sheet name="Table 6.3.2" sheetId="17" r:id="rId15"/>
-    <sheet name="T.Client.py" sheetId="15" r:id="rId16"/>
-    <sheet name="Table 6.4. Endpoints and HTTP" sheetId="20" r:id="rId17"/>
-    <sheet name="Table 6.5.1. Technologica model" sheetId="22" r:id="rId18"/>
-    <sheet name="Table 6.5.2. Medical model laye" sheetId="21" r:id="rId19"/>
-    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId20"/>
-    <sheet name="Table 7.3." sheetId="24" r:id="rId21"/>
+    <sheet name="Table 4.2." sheetId="25" r:id="rId10"/>
+    <sheet name="T.5" sheetId="11" r:id="rId11"/>
+    <sheet name="T.5.6" sheetId="12" r:id="rId12"/>
+    <sheet name="T.6 (2)" sheetId="13" r:id="rId13"/>
+    <sheet name="Table 6.3.1" sheetId="16" r:id="rId14"/>
+    <sheet name="T.Server.py" sheetId="14" r:id="rId15"/>
+    <sheet name="Table 6.3.2" sheetId="17" r:id="rId16"/>
+    <sheet name="T.Client.py" sheetId="15" r:id="rId17"/>
+    <sheet name="Table 6.4. Endpoints and HTTP" sheetId="20" r:id="rId18"/>
+    <sheet name="Table 6.5.1. Technologica model" sheetId="22" r:id="rId19"/>
+    <sheet name="Table 6.5.2. Medical model laye" sheetId="21" r:id="rId20"/>
+    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId21"/>
+    <sheet name="Table 7.3." sheetId="24" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$J$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
   </definedNames>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="375">
   <si>
     <t>FL</t>
   </si>
@@ -1388,6 +1389,27 @@
       </rPr>
       <t>"not lung."</t>
     </r>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>PySyft, FATE, Flower FedML and TensorFlow Federated</t>
+  </si>
+  <si>
+    <t>FL Frameworks</t>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>FL Datasets</t>
+  </si>
+  <si>
+    <t>Medical and Technological</t>
+  </si>
+  <si>
+    <t>RSNA Chest X-ray, MNIST and  tabular synthetic data</t>
   </si>
 </sst>
 </file>
@@ -1475,21 +1497,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1569,11 +1585,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1659,8 +1701,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1689,8 +1735,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1698,21 +1747,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2390,10 +2439,61 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892CA594-78A0-4F8B-A086-EFF2B4FB2C59}">
+  <dimension ref="E6:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="6" max="6" width="57.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:6">
+      <c r="E6" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6">
+      <c r="E7" s="52" t="s">
+        <v>370</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6">
+      <c r="E8" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6">
+      <c r="E9" s="30" t="s">
+        <v>371</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE450B4-7C85-4A17-990B-BEB82D7C7E18}">
   <dimension ref="D4:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -2470,7 +2570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251AAA7B-FC40-4F27-8AA6-A9DBE55EA49F}">
   <dimension ref="D4:O17"/>
   <sheetViews>
@@ -2490,21 +2590,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="27.6">
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="34" t="s">
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="J4" s="34"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="31"/>
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="4:15" ht="45.6" customHeight="1">
@@ -2543,7 +2643,7 @@
       <c r="E6" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="32" t="s">
         <v>193</v>
       </c>
       <c r="G6" s="22">
@@ -2572,7 +2672,7 @@
       <c r="E7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="32" t="s">
         <v>194</v>
       </c>
       <c r="G7" s="22">
@@ -2659,7 +2759,7 @@
       <c r="E10" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="32" t="s">
         <v>197</v>
       </c>
       <c r="G10" s="22">
@@ -2705,7 +2805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E6934E-D7C4-484C-AEBC-9F58A7487085}">
   <dimension ref="D4:N17"/>
   <sheetViews>
@@ -2724,13 +2824,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:14" ht="28.8">
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="41" t="s">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="41"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="1" t="s">
         <v>191</v>
       </c>
@@ -2911,7 +3011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D28749-D765-415A-9C12-E1FE75AF4B71}">
   <dimension ref="B3:C20"/>
   <sheetViews>
@@ -2933,100 +3033,100 @@
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="33" t="s">
         <v>238</v>
       </c>
       <c r="C4" s="18"/>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="33" t="s">
         <v>240</v>
       </c>
       <c r="C5" s="18"/>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="33" t="s">
         <v>242</v>
       </c>
       <c r="C6" s="18"/>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="33" t="s">
         <v>244</v>
       </c>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="33" t="s">
         <v>246</v>
       </c>
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="33" t="s">
         <v>248</v>
       </c>
       <c r="C9" s="18"/>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="33" t="s">
         <v>250</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="33" t="s">
         <v>252</v>
       </c>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="33" t="s">
         <v>254</v>
       </c>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="33" t="s">
         <v>256</v>
       </c>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="33" t="s">
         <v>258</v>
       </c>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="33" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="33" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="33" t="s">
         <v>264</v>
       </c>
       <c r="C17" s="18"/>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="33" t="s">
         <v>266</v>
       </c>
       <c r="C18" s="18"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="33" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="33" t="s">
         <v>270</v>
       </c>
     </row>
@@ -3035,7 +3135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE30FFEC-DD3A-43C2-9692-82381583DFB4}">
   <dimension ref="D3:E20"/>
   <sheetViews>
@@ -3198,7 +3298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D455F8B2-ECEE-4F97-AE0E-F30B6212FF7D}">
   <dimension ref="C3:C16"/>
   <sheetViews>
@@ -3218,67 +3318,67 @@
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="33" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="5" spans="3:3">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="33" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="33" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="7" spans="3:3">
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="33" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="8" spans="3:3">
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="33" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="9" spans="3:3">
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="33" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="10" spans="3:3">
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="33" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="11" spans="3:3">
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="33" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="12" spans="3:3">
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="33" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="33" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="14" spans="3:3">
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="33" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="15" spans="3:3">
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="33" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="16" spans="3:3">
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="33" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3287,7 +3387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1877F309-2AC0-4525-B1B7-2FED63E9E5D6}">
   <dimension ref="C3:D16"/>
   <sheetViews>
@@ -3418,7 +3518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A9E57B-1589-46D6-912B-B22AAF95984C}">
   <dimension ref="F4:K17"/>
   <sheetViews>
@@ -3456,7 +3556,7 @@
       </c>
     </row>
     <row r="5" spans="6:11">
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="33" t="s">
         <v>216</v>
       </c>
       <c r="G5" s="22" t="s">
@@ -3476,7 +3576,7 @@
       </c>
     </row>
     <row r="6" spans="6:11">
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="33" t="s">
         <v>218</v>
       </c>
       <c r="G6" s="22" t="s">
@@ -3496,7 +3596,7 @@
       </c>
     </row>
     <row r="7" spans="6:11">
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="33" t="s">
         <v>221</v>
       </c>
       <c r="G7" s="22" t="s">
@@ -3516,7 +3616,7 @@
       </c>
     </row>
     <row r="8" spans="6:11">
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="33" t="s">
         <v>220</v>
       </c>
       <c r="G8" s="22" t="s">
@@ -3536,7 +3636,7 @@
       </c>
     </row>
     <row r="9" spans="6:11">
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="33" t="s">
         <v>314</v>
       </c>
       <c r="G9" s="22" t="s">
@@ -3556,7 +3656,7 @@
       </c>
     </row>
     <row r="10" spans="6:11">
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="33" t="s">
         <v>219</v>
       </c>
       <c r="G10" s="22" t="s">
@@ -3576,7 +3676,7 @@
       </c>
     </row>
     <row r="11" spans="6:11">
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="33" t="s">
         <v>228</v>
       </c>
       <c r="G11" s="22" t="s">
@@ -3596,7 +3696,7 @@
       </c>
     </row>
     <row r="12" spans="6:11">
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="33" t="s">
         <v>229</v>
       </c>
       <c r="G12" s="22" t="s">
@@ -3616,7 +3716,7 @@
       </c>
     </row>
     <row r="13" spans="6:11">
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="33" t="s">
         <v>225</v>
       </c>
       <c r="G13" s="22" t="s">
@@ -3636,7 +3736,7 @@
       </c>
     </row>
     <row r="14" spans="6:11">
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="33" t="s">
         <v>226</v>
       </c>
       <c r="G14" s="22" t="s">
@@ -3656,7 +3756,7 @@
       </c>
     </row>
     <row r="15" spans="6:11">
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="33" t="s">
         <v>223</v>
       </c>
       <c r="G15" s="22" t="s">
@@ -3676,7 +3776,7 @@
       </c>
     </row>
     <row r="16" spans="6:11">
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="33" t="s">
         <v>222</v>
       </c>
       <c r="G16" s="22" t="s">
@@ -3696,7 +3796,7 @@
       </c>
     </row>
     <row r="17" spans="6:11">
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="33" t="s">
         <v>227</v>
       </c>
       <c r="G17" s="22" t="s">
@@ -3720,7 +3820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7298F1-C971-4635-B43B-E10502027043}">
   <dimension ref="F3:G7"/>
   <sheetViews>
@@ -3743,118 +3843,35 @@
       </c>
     </row>
     <row r="4" spans="6:7" ht="27" customHeight="1">
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="33" t="s">
         <v>318</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="33" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="5" spans="6:7" ht="27" customHeight="1">
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="33" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="6" spans="6:7" ht="27" customHeight="1">
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="33" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="7" spans="6:7" ht="27" customHeight="1">
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="33" t="s">
         <v>329</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="33" t="s">
         <v>337</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A837C353-FFBB-4CDE-9AA4-833F83C063F8}">
-  <dimension ref="D3:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
-    <col min="5" max="5" width="50.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="4:5">
-      <c r="D3" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5" ht="27.6">
-      <c r="D4" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" ht="27.6">
-      <c r="D5" s="48" t="s">
-        <v>320</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" ht="27.6">
-      <c r="D6" s="48" t="s">
-        <v>322</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" ht="41.4">
-      <c r="D7" s="48" t="s">
-        <v>324</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" ht="41.4">
-      <c r="D8" s="48" t="s">
-        <v>326</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5">
-      <c r="D9" s="48" t="s">
-        <v>330</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" ht="28.2" customHeight="1">
-      <c r="D10" s="48" t="s">
-        <v>331</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3937,6 +3954,89 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A837C353-FFBB-4CDE-9AA4-833F83C063F8}">
+  <dimension ref="D3:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="28.21875" customWidth="1"/>
+    <col min="5" max="5" width="50.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:5">
+      <c r="D3" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="27.6">
+      <c r="D4" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="27.6">
+      <c r="D5" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="27.6">
+      <c r="D6" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" ht="41.4">
+      <c r="D7" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="41.4">
+      <c r="D8" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5">
+      <c r="D9" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" ht="28.2" customHeight="1">
+      <c r="D10" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
   <sheetPr filterMode="1"/>
   <dimension ref="E3:K16"/>
@@ -4287,7 +4387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4752E1C2-D677-4722-9FF8-46C596A40F59}">
   <dimension ref="H6:M10"/>
   <sheetViews>
@@ -4306,7 +4406,7 @@
   </cols>
   <sheetData>
     <row r="6" spans="8:13" ht="43.2">
-      <c r="H6" s="49"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="1" t="s">
         <v>348</v>
       </c>
@@ -4843,25 +4943,25 @@
       </c>
     </row>
     <row r="15" spans="3:22">
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="N15" s="34" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="N15" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="34"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" t="s">
@@ -5046,11 +5146,11 @@
       </c>
     </row>
     <row r="14" spans="4:6">
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5288,11 +5388,11 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5463,19 +5563,19 @@
       <c r="E4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="5:7">
       <c r="E5" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="40" t="s">
         <v>158</v>
       </c>
     </row>
@@ -5483,31 +5583,31 @@
       <c r="E6" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="5:7">
       <c r="E7" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="5:7">
       <c r="E8" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="5:7" ht="27.6">
       <c r="E9" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5522,10 +5622,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FCD28B-1E36-4558-8911-86FA7965D0F7}">
-  <dimension ref="F6:J11"/>
+  <dimension ref="E6:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G6" sqref="G6:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5538,77 +5638,102 @@
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="7:10" ht="18" customHeight="1">
+    <row r="6" spans="5:10" ht="18" customHeight="1">
       <c r="G6" s="29" t="s">
         <v>151</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="J6" s="40"/>
-    </row>
-    <row r="7" spans="7:10">
+      <c r="J6" s="42"/>
+    </row>
+    <row r="7" spans="5:10">
       <c r="G7" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I7" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="7:10">
+    <row r="8" spans="5:10">
       <c r="G8" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="7:10" ht="27.6">
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+    </row>
+    <row r="9" spans="5:10" ht="27.6">
       <c r="G9" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="41"/>
+    </row>
+    <row r="10" spans="5:10" ht="27.6">
+      <c r="G10" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="J9" s="39"/>
-    </row>
-    <row r="10" spans="7:10" ht="27.6">
-      <c r="G10" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-    </row>
-    <row r="11" spans="7:10" ht="27.6">
+      <c r="H10" s="48" t="s">
+        <v>360</v>
+      </c>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+    </row>
+    <row r="11" spans="5:10" ht="27.6">
       <c r="G11" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>360</v>
-      </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+    </row>
+    <row r="16" spans="5:10">
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="50"/>
+    </row>
+    <row r="18" spans="5:8">
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="5:8">
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J11"/>
     <mergeCell ref="I9:I11"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Section 4. Research and Ethics Completed, Starting last section:Conclusion.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="273" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D8BBEA9-08C2-49C7-A61E-CB22AF2AF2CF}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82C9DC8B-CC63-43BE-A631-798392BB80E5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="715" firstSheet="6" activeTab="9" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="0" yWindow="528" windowWidth="13968" windowHeight="11304" tabRatio="715" firstSheet="5" activeTab="10" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -23,22 +23,23 @@
     <sheet name="T.3.6." sheetId="8" r:id="rId8"/>
     <sheet name="T.3.6.1." sheetId="10" r:id="rId9"/>
     <sheet name="Table 4.2." sheetId="25" r:id="rId10"/>
-    <sheet name="T.5" sheetId="11" r:id="rId11"/>
-    <sheet name="T.5.6" sheetId="12" r:id="rId12"/>
-    <sheet name="T.6 (2)" sheetId="13" r:id="rId13"/>
-    <sheet name="Table 6.3.1" sheetId="16" r:id="rId14"/>
-    <sheet name="T.Server.py" sheetId="14" r:id="rId15"/>
-    <sheet name="Table 6.3.2" sheetId="17" r:id="rId16"/>
-    <sheet name="T.Client.py" sheetId="15" r:id="rId17"/>
-    <sheet name="Table 6.4. Endpoints and HTTP" sheetId="20" r:id="rId18"/>
-    <sheet name="Table 6.5.1. Technologica model" sheetId="22" r:id="rId19"/>
-    <sheet name="Table 6.5.2. Medical model laye" sheetId="21" r:id="rId20"/>
-    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId21"/>
-    <sheet name="Table 7.3." sheetId="24" r:id="rId22"/>
+    <sheet name="T.4.5" sheetId="26" r:id="rId11"/>
+    <sheet name="T.5" sheetId="11" r:id="rId12"/>
+    <sheet name="T.5.6" sheetId="12" r:id="rId13"/>
+    <sheet name="T.6 (2)" sheetId="13" r:id="rId14"/>
+    <sheet name="Table 6.3.1" sheetId="16" r:id="rId15"/>
+    <sheet name="T.Server.py" sheetId="14" r:id="rId16"/>
+    <sheet name="Table 6.3.2" sheetId="17" r:id="rId17"/>
+    <sheet name="T.Client.py" sheetId="15" r:id="rId18"/>
+    <sheet name="Table 6.4. Endpoints and HTTP" sheetId="20" r:id="rId19"/>
+    <sheet name="Table 6.5.1. Technologica model" sheetId="22" r:id="rId20"/>
+    <sheet name="Table 6.5.2. Medical model laye" sheetId="21" r:id="rId21"/>
+    <sheet name="CommunicationProtocols" sheetId="18" r:id="rId22"/>
+    <sheet name="Table 7.3." sheetId="24" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$J$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
   </definedNames>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="391">
   <si>
     <t>FL</t>
   </si>
@@ -324,9 +325,6 @@
   </si>
   <si>
     <t>Convolutional Neural Network(s)</t>
-  </si>
-  <si>
-    <t>Long Short-Term Memory Networks</t>
   </si>
   <si>
     <t>LSTM(s)</t>
@@ -1121,12 +1119,6 @@
   </si>
   <si>
     <t xml:space="preserve">Null Hypothesis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shapiro Tests </t>
-  </si>
-  <si>
-    <t>ST(s)</t>
   </si>
   <si>
     <t>Clients with Improved Performance</t>
@@ -1410,6 +1402,63 @@
   </si>
   <si>
     <t>RSNA Chest X-ray, MNIST and  tabular synthetic data</t>
+  </si>
+  <si>
+    <t>OS(s)</t>
+  </si>
+  <si>
+    <t>Operating System(s)</t>
+  </si>
+  <si>
+    <t>Shapiro-Wilk Test(s)</t>
+  </si>
+  <si>
+    <t>Long Short-Term Memory Network(s)</t>
+  </si>
+  <si>
+    <t>SWT(s)</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Miro</t>
+  </si>
+  <si>
+    <t>Lucidchart</t>
+  </si>
+  <si>
+    <t>Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>Jupyter Notebook</t>
+  </si>
+  <si>
+    <t>Visual Studio Code</t>
+  </si>
+  <si>
+    <t>Notepad++</t>
+  </si>
+  <si>
+    <t>Ubuntu 22.04.4 LTS</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Windows 10 Pro/Ubutu 22.04.LTS</t>
+  </si>
+  <si>
+    <t>GitHub</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1708,6 +1757,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1735,6 +1790,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1749,19 +1810,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2101,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2123,79 +2171,79 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="19" t="s">
-        <v>342</v>
+        <v>98</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>343</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="19" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="19" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="19" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="19" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>86</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="19" t="s">
-        <v>143</v>
+        <v>4</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>144</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="19" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="19" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="19" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>36</v>
@@ -2203,58 +2251,58 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="19" t="s">
-        <v>175</v>
+        <v>78</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="19" t="s">
-        <v>83</v>
+        <v>338</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>84</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="19" t="s">
-        <v>339</v>
+        <v>0</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>338</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="19" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="19" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="19" t="s">
-        <v>89</v>
+        <v>343</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>90</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2267,18 +2315,18 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>230</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2291,26 +2339,26 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>171</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>87</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2339,58 +2387,58 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>139</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="19" t="s">
-        <v>345</v>
+        <v>372</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>344</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>340</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>149</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>141</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2403,10 +2451,10 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="19" t="s">
-        <v>346</v>
+        <v>376</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>347</v>
+        <v>374</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2425,9 +2473,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B28" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B39">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B40">
       <sortCondition ref="A1:A28"/>
     </sortState>
   </autoFilter>
@@ -2442,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892CA594-78A0-4F8B-A086-EFF2B4FB2C59}">
   <dimension ref="E6:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2454,34 +2510,34 @@
   <sheetData>
     <row r="6" spans="5:6">
       <c r="E6" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="5:6">
-      <c r="E7" s="52" t="s">
-        <v>370</v>
+      <c r="E7" s="35" t="s">
+        <v>367</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="5:6">
       <c r="E8" s="30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="5:6">
       <c r="E9" s="30" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2490,6 +2546,105 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3222-9C94-459D-9696-C9C4F2B88DE8}">
+  <dimension ref="D3:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="41.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:5">
+      <c r="D3" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5">
+      <c r="D4" s="35" t="s">
+        <v>379</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5">
+      <c r="D5" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5">
+      <c r="D6" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5">
+      <c r="D7" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5">
+      <c r="D8" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5">
+      <c r="D9" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5">
+      <c r="D10" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5">
+      <c r="D11" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5">
+      <c r="D12" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE450B4-7C85-4A17-990B-BEB82D7C7E18}">
   <dimension ref="D4:F10"/>
   <sheetViews>
@@ -2505,55 +2660,55 @@
     <row r="4" spans="4:6">
       <c r="D4" s="9"/>
       <c r="E4" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="4:6" ht="27.6">
       <c r="D5" s="10"/>
       <c r="E5" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="4:6" ht="27.6">
       <c r="D6" s="10"/>
       <c r="E6" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="4:6" ht="27.6">
       <c r="D7" s="10"/>
       <c r="E7" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="4:6" ht="27.6">
       <c r="D8" s="10"/>
       <c r="E8" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="4:6" ht="27.6">
       <c r="D9" s="10"/>
       <c r="E9" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="4:6" ht="27.6">
@@ -2562,7 +2717,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -2570,7 +2725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251AAA7B-FC40-4F27-8AA6-A9DBE55EA49F}">
   <dimension ref="D4:O17"/>
   <sheetViews>
@@ -2590,61 +2745,61 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="27.6">
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="36" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="J4" s="38"/>
+      <c r="K4" s="21" t="s">
         <v>190</v>
-      </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="21" t="s">
-        <v>191</v>
       </c>
       <c r="L4" s="31"/>
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="4:15" ht="45.6" customHeight="1">
       <c r="D5" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="F5" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="H5" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="I5" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="K5" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="L5" s="21" t="s">
         <v>182</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="6" spans="4:15">
       <c r="D6" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>58</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="22">
         <v>8</v>
@@ -2667,13 +2822,13 @@
     </row>
     <row r="7" spans="4:15">
       <c r="D7" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>42</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G7" s="22">
         <v>7</v>
@@ -2696,13 +2851,13 @@
     </row>
     <row r="8" spans="4:15" ht="41.4">
       <c r="D8" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G8" s="22">
         <v>6</v>
@@ -2725,13 +2880,13 @@
     </row>
     <row r="9" spans="4:15">
       <c r="D9" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G9" s="22">
         <v>6</v>
@@ -2754,13 +2909,13 @@
     </row>
     <row r="10" spans="4:15">
       <c r="D10" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="22">
         <v>5</v>
@@ -2805,7 +2960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E6934E-D7C4-484C-AEBC-9F58A7487085}">
   <dimension ref="D4:N17"/>
   <sheetViews>
@@ -2824,55 +2979,55 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:14" ht="28.8">
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="H4" s="47"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="51"/>
       <c r="I4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="N4" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="4:14" ht="28.8">
       <c r="D5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="4:14">
       <c r="D6" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="5">
         <v>7</v>
@@ -2891,13 +3046,13 @@
     </row>
     <row r="7" spans="4:14">
       <c r="D7" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G7" s="5">
         <v>7</v>
@@ -2916,13 +3071,13 @@
     </row>
     <row r="8" spans="4:14" ht="28.8">
       <c r="D8" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G8" s="5">
         <v>6</v>
@@ -2941,13 +3096,13 @@
     </row>
     <row r="9" spans="4:14">
       <c r="D9" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G9" s="5">
         <v>7</v>
@@ -2966,13 +3121,13 @@
     </row>
     <row r="10" spans="4:14">
       <c r="D10" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G10" s="5">
         <v>5</v>
@@ -3011,7 +3166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D28749-D765-415A-9C12-E1FE75AF4B71}">
   <dimension ref="B3:C20"/>
   <sheetViews>
@@ -3028,106 +3183,106 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="18"/>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C5" s="18"/>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" s="18"/>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" s="18"/>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17" s="18"/>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18" s="18"/>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3135,7 +3290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE30FFEC-DD3A-43C2-9692-82381583DFB4}">
   <dimension ref="D3:E20"/>
   <sheetViews>
@@ -3151,146 +3306,146 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="4:5" ht="43.2">
       <c r="D4" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>238</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="5" spans="4:5" ht="28.8">
       <c r="D5" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>240</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="28.8">
       <c r="D6" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>242</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="7" spans="4:5" ht="43.2">
       <c r="D7" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>244</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="8" spans="4:5" ht="57.6">
       <c r="D8" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="9" spans="4:5" ht="57.6">
       <c r="D9" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>248</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="57.6">
       <c r="D10" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>250</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="11" spans="4:5" ht="57.6">
       <c r="D11" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>252</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="12" spans="4:5" ht="57.6">
       <c r="D12" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>254</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="13" spans="4:5" ht="28.8">
       <c r="D13" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>256</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="14" spans="4:5" ht="28.8">
       <c r="D14" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>258</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="15" spans="4:5" ht="28.8">
       <c r="D15" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="16" spans="4:5" ht="28.8">
       <c r="D16" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>262</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="28.8">
       <c r="D17" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="57.6">
       <c r="D18" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>266</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="19" spans="4:5" ht="43.2">
       <c r="D19" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>268</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="28.8">
       <c r="D20" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3298,7 +3453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D455F8B2-ECEE-4F97-AE0E-F30B6212FF7D}">
   <dimension ref="C3:C16"/>
   <sheetViews>
@@ -3314,72 +3469,72 @@
   <sheetData>
     <row r="3" spans="3:3">
       <c r="C3" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" s="33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" s="33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" s="33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" s="33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1877F309-2AC0-4525-B1B7-2FED63E9E5D6}">
   <dimension ref="C3:D16"/>
   <sheetViews>
@@ -3403,114 +3558,114 @@
   <sheetData>
     <row r="3" spans="3:4">
       <c r="C3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="57.6">
       <c r="C4" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="43.2">
       <c r="C5" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="57.6">
       <c r="C6" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="72">
       <c r="C7" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="57.6">
       <c r="C8" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="57.6">
       <c r="C9" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="72">
       <c r="C10" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="43.2">
       <c r="C11" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="28.8">
       <c r="C12" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="57.6">
       <c r="C13" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="57.6">
       <c r="C14" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="28.8">
       <c r="C15" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="43.2">
       <c r="C16" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3518,7 +3673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A9E57B-1589-46D6-912B-B22AAF95984C}">
   <dimension ref="F4:K17"/>
   <sheetViews>
@@ -3537,341 +3692,282 @@
   <sheetData>
     <row r="4" spans="6:11" ht="27.6">
       <c r="F4" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>215</v>
-      </c>
       <c r="H4" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="21" t="s">
         <v>299</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="6:11">
       <c r="F5" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>217</v>
-      </c>
       <c r="H5" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I5" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J5" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="6:11">
       <c r="F6" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H6" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I6" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J6" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="6:11">
       <c r="F7" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="6:11">
       <c r="F8" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="6:11">
       <c r="F9" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H9" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I9" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J9" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="6:11">
       <c r="F10" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H10" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J10" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="6:11">
       <c r="F11" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I11" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="K11" s="22" t="s">
         <v>301</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="12" spans="6:11">
       <c r="F12" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I12" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="K12" s="22" t="s">
         <v>301</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="13" spans="6:11">
       <c r="F13" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H13" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I13" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J13" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="6:11">
       <c r="F14" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="6:11">
       <c r="F15" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>224</v>
-      </c>
       <c r="H15" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I15" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J15" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="6:11">
       <c r="F16" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H16" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J16" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="6:11">
       <c r="F17" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H17" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="I17" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I17" s="22" t="s">
-        <v>302</v>
-      </c>
       <c r="J17" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>301</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7298F1-C971-4635-B43B-E10502027043}">
-  <dimension ref="F3:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="60.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="6:7" ht="27" customHeight="1">
-      <c r="F3" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="6:7" ht="27" customHeight="1">
-      <c r="F4" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="6:7" ht="27" customHeight="1">
-      <c r="F5" s="33" t="s">
-        <v>333</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="6" spans="6:7" ht="27" customHeight="1">
-      <c r="F6" s="33" t="s">
-        <v>335</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="7" spans="6:7" ht="27" customHeight="1">
-      <c r="F7" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3954,6 +4050,65 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7298F1-C971-4635-B43B-E10502027043}">
+  <dimension ref="F3:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="60.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:7" ht="27" customHeight="1">
+      <c r="F3" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="6:7" ht="27" customHeight="1">
+      <c r="F4" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="6:7" ht="27" customHeight="1">
+      <c r="F5" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" ht="27" customHeight="1">
+      <c r="F6" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="6:7" ht="27" customHeight="1">
+      <c r="F7" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A837C353-FFBB-4CDE-9AA4-833F83C063F8}">
   <dimension ref="D3:E10"/>
   <sheetViews>
@@ -3969,66 +4124,66 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="4:5" ht="27.6">
       <c r="D4" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>318</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="5" spans="4:5" ht="27.6">
       <c r="D5" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>320</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="27.6">
       <c r="D6" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>322</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="7" spans="4:5" ht="41.4">
       <c r="D7" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>324</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="8" spans="4:5" ht="41.4">
       <c r="D8" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="E8" s="33" t="s">
         <v>326</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="28.2" customHeight="1">
       <c r="D10" s="33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4036,7 +4191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48E4969-AFF2-48B3-BC2C-909C74F9EEE9}">
   <sheetPr filterMode="1"/>
   <dimension ref="E3:K16"/>
@@ -4055,324 +4210,324 @@
   <sheetData>
     <row r="3" spans="5:11" ht="28.8">
       <c r="E3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="G3" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="5:11" ht="28.8">
       <c r="E4" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>217</v>
-      </c>
       <c r="G4" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>302</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="5" spans="5:11" ht="43.2">
       <c r="E5" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="5:11" ht="43.2">
       <c r="E6" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="5:11" ht="43.2">
       <c r="E7" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="5:11" ht="43.2">
       <c r="E8" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>314</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="9" spans="5:11" ht="43.2">
       <c r="E9" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="5:11" ht="43.2" hidden="1">
       <c r="E10" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="K10" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="5:11" ht="43.2" hidden="1">
       <c r="E11" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="K11" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="5:11" ht="43.2">
       <c r="E12" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="5:11" ht="28.8">
       <c r="E13" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="5:11" ht="43.2">
       <c r="E14" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>224</v>
-      </c>
       <c r="G14" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="I14" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="5:11" ht="43.2">
       <c r="E15" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="I15" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="5:11" ht="43.2">
       <c r="E16" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="I16" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4387,7 +4542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4752E1C2-D677-4722-9FF8-46C596A40F59}">
   <dimension ref="H6:M10"/>
   <sheetViews>
@@ -4408,24 +4563,24 @@
     <row r="6" spans="8:13" ht="43.2">
       <c r="H6" s="7"/>
       <c r="I6" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="7" spans="8:13">
       <c r="H7" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I7" s="5">
         <v>2</v>
@@ -4437,15 +4592,15 @@
         <v>0</v>
       </c>
       <c r="L7" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="8" spans="8:13">
       <c r="H8" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I8" s="5">
         <v>3</v>
@@ -4457,15 +4612,15 @@
         <v>0</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="8:13">
       <c r="H9" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -4477,15 +4632,15 @@
         <v>5</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="8:13">
       <c r="H10" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>
@@ -4497,10 +4652,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4943,25 +5098,25 @@
       </c>
     </row>
     <row r="15" spans="3:22">
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="N15" s="36" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="N15" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38"/>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" t="s">
@@ -5146,11 +5301,11 @@
       </c>
     </row>
     <row r="14" spans="4:6">
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5179,10 +5334,10 @@
   <sheetData>
     <row r="5" spans="5:6">
       <c r="E5" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="5:6" ht="55.2">
@@ -5190,15 +5345,15 @@
         <v>78</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="5:6" ht="55.2">
       <c r="E7" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="5:6" ht="55.2">
@@ -5206,15 +5361,15 @@
         <v>83</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="5:6" ht="55.2">
       <c r="E9" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" spans="5:6">
@@ -5250,7 +5405,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="G2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>37</v>
@@ -5263,7 +5418,7 @@
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="G3" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" s="22" t="s">
         <v>45</v>
@@ -5276,7 +5431,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="G4" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="22" t="s">
         <v>44</v>
@@ -5289,7 +5444,7 @@
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="G5" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>42</v>
@@ -5302,7 +5457,7 @@
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="G6" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" s="22" t="s">
         <v>58</v>
@@ -5315,7 +5470,7 @@
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="G7" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" s="22" t="s">
         <v>9</v>
@@ -5328,7 +5483,7 @@
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="G8" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>46</v>
@@ -5341,7 +5496,7 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="G9" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H9" s="22" t="s">
         <v>41</v>
@@ -5354,7 +5509,7 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="G10" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>56</v>
@@ -5367,7 +5522,7 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="G11" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>43</v>
@@ -5378,7 +5533,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="G12" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H12" s="22" t="s">
         <v>47</v>
@@ -5388,11 +5543,11 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5421,122 +5576,122 @@
   <sheetData>
     <row r="3" spans="6:7">
       <c r="F3" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>112</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="6:7" ht="27.6">
       <c r="F4" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="6:7">
       <c r="F5" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="6" spans="6:7">
       <c r="F6" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>117</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="6:7">
       <c r="F7" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="6:7">
       <c r="F8" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9" spans="6:7">
       <c r="F9" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="10" spans="6:7">
       <c r="F10" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="6:7" ht="55.2">
       <c r="F11" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="6:7" ht="27.6">
       <c r="F12" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" spans="6:7">
       <c r="F13" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="28" t="s">
         <v>129</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="14" spans="6:7" ht="41.4">
       <c r="F14" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>131</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="15" spans="6:7" ht="28.2">
       <c r="F15" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="6:7" ht="27.6">
       <c r="F16" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="6:7">
       <c r="F17" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -5561,53 +5716,53 @@
   <sheetData>
     <row r="4" spans="5:7">
       <c r="E4" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="G4" s="36"/>
+        <v>150</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="5:7">
       <c r="E5" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="42" t="s">
         <v>158</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="5:7">
       <c r="E6" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+        <v>152</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="5:7">
       <c r="E7" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="40"/>
+        <v>153</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="42"/>
     </row>
     <row r="8" spans="5:7">
       <c r="E8" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+        <v>154</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="5:7" ht="27.6">
       <c r="E9" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+        <v>155</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5622,7 +5777,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FCD28B-1E36-4558-8911-86FA7965D0F7}">
-  <dimension ref="E6:J19"/>
+  <dimension ref="F6:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6:J11"/>
@@ -5638,93 +5793,72 @@
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:10" ht="18" customHeight="1">
+    <row r="6" spans="7:10" ht="18" customHeight="1">
       <c r="G6" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="44"/>
+    </row>
+    <row r="7" spans="7:10">
+      <c r="G7" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H7" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="I6" s="42" t="s">
-        <v>160</v>
-      </c>
-      <c r="J6" s="42"/>
-    </row>
-    <row r="7" spans="5:10">
-      <c r="G7" s="29" t="s">
+      <c r="I7" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="7:10">
+      <c r="G8" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+    </row>
+    <row r="9" spans="7:10" ht="27.6">
+      <c r="G9" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="5:10">
-      <c r="G8" s="29" t="s">
+      <c r="I9" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="J9" s="43"/>
+    </row>
+    <row r="10" spans="7:10" ht="27.6">
+      <c r="G10" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-    </row>
-    <row r="9" spans="5:10" ht="27.6">
-      <c r="G9" s="29" t="s">
+      <c r="H10" s="45" t="s">
+        <v>357</v>
+      </c>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" spans="7:10" ht="27.6">
+      <c r="G11" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="J9" s="41"/>
-    </row>
-    <row r="10" spans="5:10" ht="27.6">
-      <c r="G10" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-    </row>
-    <row r="11" spans="5:10" ht="27.6">
-      <c r="G11" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="H11" s="49"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="16" spans="5:10">
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-    </row>
-    <row r="17" spans="5:8">
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="50"/>
-    </row>
-    <row r="18" spans="5:8">
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-    </row>
-    <row r="19" spans="5:8">
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Conclusion completed, 482 words left for the abstract.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82C9DC8B-CC63-43BE-A631-798392BB80E5}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F13A2843-3A2B-46C2-AB24-A3F39566C358}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="528" windowWidth="13968" windowHeight="11304" tabRatio="715" firstSheet="5" activeTab="10" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="715" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <sheet name="Table 7.3." sheetId="24" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">CommunicationProtocols!$E$3:$K$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$J$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="392">
   <si>
     <t>FL</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t xml:space="preserve">Distributed Machine Learning </t>
-  </si>
-  <si>
-    <t>FC</t>
   </si>
   <si>
     <t>Federated Core</t>
@@ -1459,6 +1456,12 @@
   </si>
   <si>
     <t>GitHub</t>
+  </si>
+  <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>Hypertext Transfer Protocol Secure</t>
   </si>
 </sst>
 </file>
@@ -2151,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2171,42 +2174,42 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>172</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2219,10 +2222,10 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2235,98 +2238,98 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="19" t="s">
-        <v>174</v>
+        <v>77</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="19" t="s">
-        <v>83</v>
+        <v>337</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>84</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="19" t="s">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>337</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="19" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="19" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="19" t="s">
-        <v>88</v>
+        <v>342</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>89</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="19" t="s">
-        <v>343</v>
+        <v>14</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>344</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="19" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>15</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="19" t="s">
-        <v>231</v>
+        <v>390</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>234</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2339,26 +2342,26 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2371,10 +2374,10 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2387,74 +2390,74 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>138</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>372</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>146</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>339</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>140</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2475,20 +2478,20 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B28" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
+  <autoFilter ref="A1:B27" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B40">
-      <sortCondition ref="A1:A28"/>
+      <sortCondition ref="A1:A27"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B30">
-    <sortCondition ref="A2:A30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
+    <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2510,34 +2513,34 @@
   <sheetData>
     <row r="6" spans="5:6">
       <c r="E6" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="5:6">
       <c r="E7" s="35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="5:6">
       <c r="E8" s="30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="5:6">
       <c r="E9" s="30" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2549,7 +2552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3222-9C94-459D-9696-C9C4F2B88DE8}">
   <dimension ref="D3:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -2561,82 +2564,82 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" s="29" t="s">
+        <v>376</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>377</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="4" spans="4:5">
       <c r="D4" s="35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="4:5">
       <c r="D5" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="4:5">
       <c r="D6" s="30" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="4:5">
       <c r="D7" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>382</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="8" spans="4:5">
       <c r="D8" s="30" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="4:5">
       <c r="D10" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>386</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="11" spans="4:5">
       <c r="D11" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>388</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="12" spans="4:5">
       <c r="D12" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -2660,55 +2663,55 @@
     <row r="4" spans="4:6">
       <c r="D4" s="9"/>
       <c r="E4" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>163</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" spans="4:6" ht="27.6">
       <c r="D5" s="10"/>
       <c r="E5" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="4:6" ht="27.6">
       <c r="D6" s="10"/>
       <c r="E6" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="4:6" ht="27.6">
       <c r="D7" s="10"/>
       <c r="E7" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="4:6" ht="27.6">
       <c r="D8" s="10"/>
       <c r="E8" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="4:6" ht="27.6">
       <c r="D9" s="10"/>
       <c r="E9" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="4:6" ht="27.6">
@@ -2717,7 +2720,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2749,57 +2752,57 @@
       <c r="E4" s="47"/>
       <c r="F4" s="48"/>
       <c r="G4" s="38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H4" s="38"/>
       <c r="I4" s="38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J4" s="38"/>
       <c r="K4" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L4" s="31"/>
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="4:15" ht="45.6" customHeight="1">
       <c r="D5" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="F5" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="H5" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="I5" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="K5" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="L5" s="21" t="s">
         <v>181</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="6" spans="4:15">
       <c r="D6" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G6" s="22">
         <v>8</v>
@@ -2822,13 +2825,13 @@
     </row>
     <row r="7" spans="4:15">
       <c r="D7" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G7" s="22">
         <v>7</v>
@@ -2851,13 +2854,13 @@
     </row>
     <row r="8" spans="4:15" ht="41.4">
       <c r="D8" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="22">
         <v>6</v>
@@ -2880,13 +2883,13 @@
     </row>
     <row r="9" spans="4:15">
       <c r="D9" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G9" s="22">
         <v>6</v>
@@ -2909,13 +2912,13 @@
     </row>
     <row r="10" spans="4:15">
       <c r="D10" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G10" s="22">
         <v>5</v>
@@ -2983,51 +2986,51 @@
       <c r="E4" s="49"/>
       <c r="F4" s="50"/>
       <c r="G4" s="51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H4" s="51"/>
       <c r="I4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="N4" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="4:14" ht="28.8">
       <c r="D5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="4:14">
       <c r="D6" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G6" s="5">
         <v>7</v>
@@ -3046,13 +3049,13 @@
     </row>
     <row r="7" spans="4:14">
       <c r="D7" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G7" s="5">
         <v>7</v>
@@ -3071,13 +3074,13 @@
     </row>
     <row r="8" spans="4:14" ht="28.8">
       <c r="D8" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="5">
         <v>6</v>
@@ -3096,13 +3099,13 @@
     </row>
     <row r="9" spans="4:14">
       <c r="D9" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G9" s="5">
         <v>7</v>
@@ -3121,13 +3124,13 @@
     </row>
     <row r="10" spans="4:14">
       <c r="D10" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G10" s="5">
         <v>5</v>
@@ -3183,106 +3186,106 @@
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C4" s="18"/>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C5" s="18"/>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C6" s="18"/>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C9" s="18"/>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17" s="18"/>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C18" s="18"/>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3306,146 +3309,146 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="4:5" ht="43.2">
       <c r="D4" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>237</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="4:5" ht="28.8">
       <c r="D5" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>239</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="28.8">
       <c r="D6" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>241</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="7" spans="4:5" ht="43.2">
       <c r="D7" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>243</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="8" spans="4:5" ht="57.6">
       <c r="D8" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>245</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="9" spans="4:5" ht="57.6">
       <c r="D9" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>247</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="57.6">
       <c r="D10" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="11" spans="4:5" ht="57.6">
       <c r="D11" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>251</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="12" spans="4:5" ht="57.6">
       <c r="D12" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>253</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="13" spans="4:5" ht="28.8">
       <c r="D13" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>255</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="14" spans="4:5" ht="28.8">
       <c r="D14" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>257</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="15" spans="4:5" ht="28.8">
       <c r="D15" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>259</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="16" spans="4:5" ht="28.8">
       <c r="D16" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>261</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="28.8">
       <c r="D17" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>263</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="57.6">
       <c r="D18" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>265</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="19" spans="4:5" ht="43.2">
       <c r="D19" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>267</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="28.8">
       <c r="D20" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>269</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3469,72 +3472,72 @@
   <sheetData>
     <row r="3" spans="3:3">
       <c r="C3" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" s="33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" s="33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3558,114 +3561,114 @@
   <sheetData>
     <row r="3" spans="3:4">
       <c r="C3" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="57.6">
       <c r="C4" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="43.2">
       <c r="C5" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="57.6">
       <c r="C6" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="72">
       <c r="C7" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="57.6">
       <c r="C8" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="57.6">
       <c r="C9" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="72">
       <c r="C10" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="43.2">
       <c r="C11" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="28.8">
       <c r="C12" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="57.6">
       <c r="C13" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="57.6">
       <c r="C14" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="28.8">
       <c r="C15" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="43.2">
       <c r="C16" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3692,282 +3695,282 @@
   <sheetData>
     <row r="4" spans="6:11" ht="27.6">
       <c r="F4" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>214</v>
-      </c>
       <c r="H4" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="I4" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="21" t="s">
         <v>298</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="5" spans="6:11">
       <c r="F5" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>216</v>
-      </c>
       <c r="H5" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I5" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J5" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="6:11">
       <c r="F6" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H6" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I6" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J6" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="6:11">
       <c r="F7" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="6:11">
       <c r="F8" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="6:11">
       <c r="F9" s="33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H9" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I9" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J9" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="6:11">
       <c r="F10" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H10" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J10" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="6:11">
       <c r="F11" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I11" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="K11" s="22" t="s">
         <v>300</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="12" spans="6:11">
       <c r="F12" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I12" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="K12" s="22" t="s">
         <v>300</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="13" spans="6:11">
       <c r="F13" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H13" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I13" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J13" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="6:11">
       <c r="F14" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="6:11">
       <c r="F15" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>223</v>
-      </c>
       <c r="H15" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I15" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J15" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="6:11">
       <c r="F16" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H16" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J16" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="6:11">
       <c r="F17" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H17" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="I17" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I17" s="22" t="s">
-        <v>301</v>
-      </c>
       <c r="J17" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -4065,42 +4068,42 @@
   <sheetData>
     <row r="3" spans="6:7" ht="27" customHeight="1">
       <c r="F3" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="6:7" ht="27" customHeight="1">
       <c r="F4" s="33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="6:7" ht="27" customHeight="1">
       <c r="F5" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="G5" s="33" t="s">
         <v>332</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="6" spans="6:7" ht="27" customHeight="1">
       <c r="F6" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>334</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="7" spans="6:7" ht="27" customHeight="1">
       <c r="F7" s="33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -4124,66 +4127,66 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="4:5" ht="27.6">
       <c r="D4" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>317</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="5" spans="4:5" ht="27.6">
       <c r="D5" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>319</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="27.6">
       <c r="D6" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>321</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="7" spans="4:5" ht="41.4">
       <c r="D7" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>323</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="8" spans="4:5" ht="41.4">
       <c r="D8" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="E8" s="33" t="s">
         <v>325</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="9" spans="4:5">
       <c r="D9" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="28.2" customHeight="1">
       <c r="D10" s="33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -4210,324 +4213,324 @@
   <sheetData>
     <row r="3" spans="5:11" ht="28.8">
       <c r="E3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="G3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="5:11" ht="28.8">
       <c r="E4" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="G4" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>301</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="5" spans="5:11" ht="43.2">
       <c r="E5" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="5:11" ht="43.2">
       <c r="E6" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="5:11" ht="43.2">
       <c r="E7" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="5:11" ht="43.2">
       <c r="E8" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="9" spans="5:11" ht="43.2">
       <c r="E9" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="5:11" ht="43.2" hidden="1">
       <c r="E10" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="K10" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="5:11" ht="43.2" hidden="1">
       <c r="E11" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="K11" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="5:11" ht="43.2">
       <c r="E12" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="5:11" ht="28.8">
       <c r="E13" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="5:11" ht="43.2">
       <c r="E14" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="G14" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="I14" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="5:11" ht="43.2">
       <c r="E15" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="I15" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="5:11" ht="43.2">
       <c r="E16" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>301</v>
-      </c>
       <c r="I16" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4563,24 +4566,24 @@
     <row r="6" spans="8:13" ht="43.2">
       <c r="H6" s="7"/>
       <c r="I6" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="7" spans="8:13">
       <c r="H7" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I7" s="5">
         <v>2</v>
@@ -4592,15 +4595,15 @@
         <v>0</v>
       </c>
       <c r="L7" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="8" spans="8:13">
       <c r="H8" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I8" s="5">
         <v>3</v>
@@ -4612,15 +4615,15 @@
         <v>0</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="8:13">
       <c r="H9" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -4632,15 +4635,15 @@
         <v>5</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="8:13">
       <c r="H10" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>
@@ -4652,10 +4655,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -4700,31 +4703,31 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="N4" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="P4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="Q4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="R4" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="R4" s="21" t="s">
-        <v>68</v>
-      </c>
       <c r="S4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="21" t="s">
-        <v>39</v>
-      </c>
       <c r="V4" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="3:22">
@@ -4737,7 +4740,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="N5" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O5" s="23">
         <v>1</v>
@@ -4761,7 +4764,7 @@
         <v>429</v>
       </c>
       <c r="V5" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="3:22">
@@ -4774,7 +4777,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="N6" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O6" s="23">
         <v>0.51295007204140897</v>
@@ -4798,7 +4801,7 @@
         <v>86</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="3:22">
@@ -4811,7 +4814,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="N7" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O7" s="23">
         <v>0.37812447550218559</v>
@@ -4835,7 +4838,7 @@
         <v>127</v>
       </c>
       <c r="V7" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="3:22">
@@ -4848,7 +4851,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="N8" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O8" s="23">
         <v>0.31170466209765263</v>
@@ -4872,7 +4875,7 @@
         <v>66</v>
       </c>
       <c r="V8" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="3:22">
@@ -4909,7 +4912,7 @@
         <v>108</v>
       </c>
       <c r="V9" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="3:22">
@@ -4922,7 +4925,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="N10" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O10" s="23">
         <v>9.9274705123282195E-2</v>
@@ -4946,7 +4949,7 @@
         <v>83</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="3:22">
@@ -4959,7 +4962,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="N11" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O11" s="23">
         <v>5.7416181202695593E-2</v>
@@ -4983,7 +4986,7 @@
         <v>40</v>
       </c>
       <c r="V11" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="3:22">
@@ -4996,7 +4999,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="N12" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O12" s="23">
         <v>3.601054449160878E-2</v>
@@ -5020,7 +5023,7 @@
         <v>25</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="3:22">
@@ -5033,7 +5036,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="N13" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O13" s="23">
         <v>2.1428571428571425E-2</v>
@@ -5057,7 +5060,7 @@
         <v>36</v>
       </c>
       <c r="V13" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="3:22">
@@ -5070,7 +5073,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="N14" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O14" s="23">
         <v>1.7409318218831567E-2</v>
@@ -5094,7 +5097,7 @@
         <v>9</v>
       </c>
       <c r="V14" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="3:22">
@@ -5107,7 +5110,7 @@
       <c r="I15" s="37"/>
       <c r="J15" s="37"/>
       <c r="N15" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
@@ -5120,7 +5123,7 @@
     </row>
     <row r="18" spans="3:6">
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <f>MIN(D5:D14)</f>
@@ -5137,7 +5140,7 @@
     </row>
     <row r="19" spans="3:6">
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <f>MAX(D5:D14)</f>
@@ -5181,128 +5184,128 @@
   <sheetData>
     <row r="3" spans="4:6">
       <c r="D3" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="4:6">
       <c r="D4" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="4:6">
       <c r="D5" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="4:6">
       <c r="D6" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="4:6">
       <c r="D7" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>47</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="4:6">
       <c r="D8" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="4:6">
       <c r="D9" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="4:6">
       <c r="D10" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="4:6">
       <c r="D11" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="4:6" ht="27.6">
       <c r="D12" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="4:6" ht="27.6">
       <c r="D13" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>56</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="4:6">
       <c r="D14" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" s="40"/>
       <c r="F14" s="41"/>
@@ -5334,42 +5337,42 @@
   <sheetData>
     <row r="5" spans="5:6">
       <c r="E5" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="5:6" ht="55.2">
       <c r="E6" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="5:6" ht="55.2">
       <c r="E7" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="5:6" ht="55.2">
       <c r="E8" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="5:6" ht="55.2">
       <c r="E9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="5:6">
@@ -5405,146 +5408,146 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="G2" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="G3" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="33.6" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="G4" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="G5" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="G6" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="G7" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="G8" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="G9" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="G10" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="G11" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="G12" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="28" t="s">
         <v>47</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="G13" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="40"/>
       <c r="I13" s="41"/>
@@ -5576,122 +5579,122 @@
   <sheetData>
     <row r="3" spans="6:7">
       <c r="F3" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="6:7" ht="27.6">
       <c r="F4" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="6:7">
       <c r="F5" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>114</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="6:7">
       <c r="F6" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>116</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="6:7">
       <c r="F7" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="6:7">
       <c r="F8" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>120</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="6:7">
       <c r="F9" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="10" spans="6:7">
       <c r="F10" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="6:7" ht="55.2">
       <c r="F11" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="6:7" ht="27.6">
       <c r="F12" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>126</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="13" spans="6:7">
       <c r="F13" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="28" t="s">
         <v>128</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="14" spans="6:7" ht="41.4">
       <c r="F14" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="6:7" ht="28.2">
       <c r="F15" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="6:7" ht="27.6">
       <c r="F16" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="6:7">
       <c r="F17" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -5716,50 +5719,50 @@
   <sheetData>
     <row r="4" spans="5:7">
       <c r="E4" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G4" s="38"/>
     </row>
     <row r="5" spans="5:7">
       <c r="E5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="5:7">
       <c r="E6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
     </row>
     <row r="7" spans="5:7">
       <c r="E7" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G7" s="42"/>
     </row>
     <row r="8" spans="5:7">
       <c r="E8" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
     </row>
     <row r="9" spans="5:7" ht="27.6">
       <c r="E9" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
@@ -5795,33 +5798,33 @@
   <sheetData>
     <row r="6" spans="7:10" ht="18" customHeight="1">
       <c r="G6" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J6" s="44"/>
     </row>
     <row r="7" spans="7:10">
       <c r="G7" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H7" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="7:10">
       <c r="G8" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
@@ -5829,29 +5832,29 @@
     </row>
     <row r="9" spans="7:10" ht="27.6">
       <c r="G9" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I9" s="43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J9" s="43"/>
     </row>
     <row r="10" spans="7:10" ht="27.6">
       <c r="G10" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" s="45" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
     </row>
     <row r="11" spans="7:10" ht="27.6">
       <c r="G11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H11" s="46"/>
       <c r="I11" s="43"/>

</xml_diff>

<commit_message>
Last commit, all set for grading 27-09-2024.
</commit_message>
<xml_diff>
--- a/FiguresAndTables/AbbreviationsAndTables.xlsx
+++ b/FiguresAndTables/AbbreviationsAndTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/Capstone_MScData_Sept23_SB/FiguresAndTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="676" documentId="14_{9C6F5839-6F14-470A-8A8C-2773A6D0C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{510711AF-1EAE-4E3D-9619-B09F23FC6E6A}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="14_{B8BE56AF-D41F-45DF-A829-7B7F93141A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E235864F-34AA-4380-9C26-8BB5CC3BF8C7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="942" firstSheet="4" activeTab="10" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
+    <workbookView xWindow="28815" yWindow="0" windowWidth="13755" windowHeight="15495" tabRatio="942" xr2:uid="{C3A91DCB-50E1-4673-830B-69474B35E162}"/>
   </bookViews>
   <sheets>
     <sheet name="Abbreviations" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <sheet name="T.10.4.4" sheetId="34" r:id="rId30"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abbreviations!$A$1:$B$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'T.10.2.3'!$E$3:$K$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'T.3.1.'!$C$4:$J$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'T.3.2.'!$D$3:$F$13</definedName>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="442">
   <si>
     <t>FL</t>
   </si>
@@ -1616,6 +1616,9 @@
   </si>
   <si>
     <t>Overleaf (LaTeX Editor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Independent and Identically Distributed </t>
   </si>
 </sst>
 </file>
@@ -2009,10 +2012,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2330,15 +2329,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2512,160 +2511,168 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>12</v>
+        <v>417</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>13</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>169</v>
+        <v>12</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>170</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>228</v>
+        <v>169</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>368</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>3</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
-        <v>365</v>
+        <v>137</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>366</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>145</v>
+        <v>365</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>146</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>227</v>
+        <v>145</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>230</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
-        <v>332</v>
+        <v>227</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>333</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>147</v>
+        <v>332</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>148</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
-        <v>369</v>
+        <v>69</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>367</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
-        <v>8</v>
+        <v>369</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>9</v>
+        <v>367</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B41" s="15" t="s">
         <v>334</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B27" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B40">
-      <sortCondition ref="A1:A27"/>
+  <autoFilter ref="A1:B26" xr:uid="{C909BF2B-16FF-4C17-83EE-699C534C442A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
+      <sortCondition ref="A1:A26"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
@@ -2730,7 +2737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3222-9C94-459D-9696-C9C4F2B88DE8}">
   <dimension ref="D3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>